<commit_message>
Belgium data, ability to skip links, some others
</commit_message>
<xml_diff>
--- a/a-place-for-salvador-allende/a_place_for_salvador_allende.xlsx
+++ b/a-place-for-salvador-allende/a_place_for_salvador_allende.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://onemsci-my.sharepoint.com/personal/glo_canonoy_msci_com/Documents/03 Training/datasets-of-interest/a-place-for-salvador-allende/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1693" documentId="11_FF6F299C653B866D72320E251CEDB2C4009A2F63" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31F8020B-B8CC-470C-A63E-20BAE5375DDD}"/>
+  <xr:revisionPtr revIDLastSave="1701" documentId="11_FF6F299C653B866D72320E251CEDB2C4009A2F63" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA12BCC1-DDAF-4DBE-AE5B-B8CD9F9A39AA}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2427" uniqueCount="1267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2609" uniqueCount="1351">
   <si>
     <t>id</t>
   </si>
@@ -4038,6 +4038,269 @@
   <si>
     <t>Rua Salvador Allende
 Presidente do Chile de 1970 a 1973</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>Wallonia</t>
+  </si>
+  <si>
+    <t>Liège</t>
+  </si>
+  <si>
+    <t>Wandre</t>
+  </si>
+  <si>
+    <t>4020</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/90882847</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/wcUyq3FWKnTq8cFV9</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2013/10/05/618-provincia-de-liege-belgica</t>
+  </si>
+  <si>
+    <t>Square Allende</t>
+  </si>
+  <si>
+    <t>Seraing</t>
+  </si>
+  <si>
+    <t>Boncelles</t>
+  </si>
+  <si>
+    <t>Le Bol d'Air</t>
+  </si>
+  <si>
+    <t>4102</t>
+  </si>
+  <si>
+    <t>Hommage à 
+Salvador Allende
+Président démocratique du Chili
+Assassiné le 11 septembre 1973</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/43156317</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/Qk6NPB9umkiNK4Yk7</t>
+  </si>
+  <si>
+    <t>Fléron</t>
+  </si>
+  <si>
+    <t>Romsée</t>
+  </si>
+  <si>
+    <t>4624</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/29344071</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/ZkgGBErYHpbrE7yW9</t>
+  </si>
+  <si>
+    <t>Beyne-Heusay</t>
+  </si>
+  <si>
+    <t>Queue-du-Bois</t>
+  </si>
+  <si>
+    <t>Moulins-sous-Fléron</t>
+  </si>
+  <si>
+    <t>4610</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/55696733</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/aEd4JhSLWuprJimf9</t>
+  </si>
+  <si>
+    <t>Square Salvador Allende - Salvador Allende Square</t>
+  </si>
+  <si>
+    <t>Brussels-Capital</t>
+  </si>
+  <si>
+    <t>Brussels</t>
+  </si>
+  <si>
+    <t>Pentagon</t>
+  </si>
+  <si>
+    <t>Marolles - Marollen</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>Ville de Bruxelles
+Square Salvador Allende
+Président de la République du Chili
+26 juin 1908 - 11 septembre 1973
+Stad Brussel
+Square Salvador Allende
+President van de Chileense Republiek
+26 juni 1908 - 11 september 1973</t>
+  </si>
+  <si>
+    <t>fr, nl</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/29562164</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/YT9ymKgNmRZzStse9</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2012/09/17/594-bruselas-belgica</t>
+  </si>
+  <si>
+    <t>Salle Allende - Art contemporain</t>
+  </si>
+  <si>
+    <t>Solbosch - Solbos</t>
+  </si>
+  <si>
+    <t>24, Avenue Paul Héger - Paul Hégerlaan</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/node/2465448020</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/T8eqsnxXxj6N9wfE6</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2010/02/12/472-bruselas-belgica</t>
+  </si>
+  <si>
+    <t>Salvador Allende, monumento</t>
+  </si>
+  <si>
+    <t>Flobecq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La historia es nuestra y la hacen los pueblos. Salvador Allende 1908 - 1973
+</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/129256529</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/xBrbQzNMymREspfGA</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2008/03/10/160-flobecq-belgica</t>
+  </si>
+  <si>
+    <t>Place Salvador Allende - Salvador Allendeplein</t>
+  </si>
+  <si>
+    <t>Evere</t>
+  </si>
+  <si>
+    <t>1140</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/FApGcBztWMYFv4Wi8</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2007/09/15/95-evere-belgica</t>
+  </si>
+  <si>
+    <t>Ans</t>
+  </si>
+  <si>
+    <t>4430</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/118965913</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/a1G37ZiYep2xt9Ax9</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2007/02/18/27-belgica</t>
+  </si>
+  <si>
+    <t>Hainaut</t>
+  </si>
+  <si>
+    <t>Mons</t>
+  </si>
+  <si>
+    <t>Havré</t>
+  </si>
+  <si>
+    <t>Beaulieu</t>
+  </si>
+  <si>
+    <t>7021</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/314601818</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/brnviUGJE6sERpnY9</t>
+  </si>
+  <si>
+    <t>La Louvière</t>
+  </si>
+  <si>
+    <t>Binche</t>
+  </si>
+  <si>
+    <t>Leval-Trahegnies</t>
+  </si>
+  <si>
+    <t>7134</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/333397818</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/dw4chhNvNVxmwtuQA</t>
+  </si>
+  <si>
+    <t>Charleroi</t>
+  </si>
+  <si>
+    <t>Courcelles</t>
+  </si>
+  <si>
+    <t>Souvret</t>
+  </si>
+  <si>
+    <t>6180</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/node/3714120118</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/L2uayExqRV69zA5g8</t>
+  </si>
+  <si>
+    <t>Ath</t>
+  </si>
+  <si>
+    <t>Maffle</t>
+  </si>
+  <si>
+    <t>7810</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/460056820</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/VcEeq2wFxMWqPRLy6</t>
   </si>
 </sst>
 </file>
@@ -4372,13 +4635,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AO199"/>
+  <dimension ref="A1:AO213"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B177" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B195" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H202" sqref="H202"/>
+      <selection pane="bottomRight" activeCell="A214" sqref="A214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -16789,6 +17052,847 @@
       </c>
       <c r="Y199" s="3" t="s">
         <v>1207</v>
+      </c>
+    </row>
+    <row r="200" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A200" s="3">
+        <v>199</v>
+      </c>
+      <c r="B200" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="C200" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D200" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="E200" s="3" t="s">
+        <v>1267</v>
+      </c>
+      <c r="F200" s="3" t="s">
+        <v>1268</v>
+      </c>
+      <c r="G200" s="3" t="s">
+        <v>1269</v>
+      </c>
+      <c r="H200" s="3" t="s">
+        <v>1270</v>
+      </c>
+      <c r="K200" s="10" t="s">
+        <v>1271</v>
+      </c>
+      <c r="L200" s="3">
+        <v>50.661005400000001</v>
+      </c>
+      <c r="M200" s="3">
+        <v>5.6601423000000004</v>
+      </c>
+      <c r="N200" s="3">
+        <v>2009</v>
+      </c>
+      <c r="O200" s="3">
+        <v>7</v>
+      </c>
+      <c r="Q200" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="V200" s="3">
+        <v>1</v>
+      </c>
+      <c r="W200" s="3" t="s">
+        <v>1272</v>
+      </c>
+      <c r="X200" s="3" t="s">
+        <v>1273</v>
+      </c>
+      <c r="Y200" s="3" t="s">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="201" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A201" s="3">
+        <v>200</v>
+      </c>
+      <c r="B201" s="3" t="s">
+        <v>1275</v>
+      </c>
+      <c r="C201" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D201" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="E201" s="3" t="s">
+        <v>1267</v>
+      </c>
+      <c r="F201" s="3" t="s">
+        <v>1268</v>
+      </c>
+      <c r="G201" s="3" t="s">
+        <v>1269</v>
+      </c>
+      <c r="H201" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="I201" s="3" t="s">
+        <v>1277</v>
+      </c>
+      <c r="J201" s="3" t="s">
+        <v>1278</v>
+      </c>
+      <c r="K201" s="10" t="s">
+        <v>1279</v>
+      </c>
+      <c r="L201" s="3">
+        <v>50.578284099999998</v>
+      </c>
+      <c r="M201" s="3">
+        <v>5.5435295</v>
+      </c>
+      <c r="N201" s="3">
+        <v>2009</v>
+      </c>
+      <c r="O201" s="3">
+        <v>5</v>
+      </c>
+      <c r="Q201" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="R201" s="3" t="s">
+        <v>1280</v>
+      </c>
+      <c r="S201" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="V201" s="3">
+        <v>1</v>
+      </c>
+      <c r="W201" s="3" t="s">
+        <v>1281</v>
+      </c>
+      <c r="X201" s="3" t="s">
+        <v>1282</v>
+      </c>
+      <c r="Y201" s="3" t="s">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="202" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A202" s="3">
+        <v>201</v>
+      </c>
+      <c r="B202" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="C202" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D202" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="E202" s="3" t="s">
+        <v>1267</v>
+      </c>
+      <c r="F202" s="3" t="s">
+        <v>1268</v>
+      </c>
+      <c r="G202" s="3" t="s">
+        <v>1269</v>
+      </c>
+      <c r="H202" s="3" t="s">
+        <v>1283</v>
+      </c>
+      <c r="I202" s="3" t="s">
+        <v>1284</v>
+      </c>
+      <c r="K202" s="10" t="s">
+        <v>1285</v>
+      </c>
+      <c r="L202" s="3">
+        <v>50.6116788</v>
+      </c>
+      <c r="M202" s="3">
+        <v>5.6718361000000002</v>
+      </c>
+      <c r="N202" s="3">
+        <v>2009</v>
+      </c>
+      <c r="O202" s="3">
+        <v>6</v>
+      </c>
+      <c r="Q202" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="V202" s="3">
+        <v>1</v>
+      </c>
+      <c r="W202" s="3" t="s">
+        <v>1286</v>
+      </c>
+      <c r="X202" s="3" t="s">
+        <v>1287</v>
+      </c>
+      <c r="Y202" s="3" t="s">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="203" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A203" s="3">
+        <v>202</v>
+      </c>
+      <c r="B203" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="C203" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D203" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="E203" s="3" t="s">
+        <v>1267</v>
+      </c>
+      <c r="F203" s="3" t="s">
+        <v>1268</v>
+      </c>
+      <c r="G203" s="3" t="s">
+        <v>1269</v>
+      </c>
+      <c r="H203" s="3" t="s">
+        <v>1288</v>
+      </c>
+      <c r="I203" s="3" t="s">
+        <v>1289</v>
+      </c>
+      <c r="J203" s="3" t="s">
+        <v>1290</v>
+      </c>
+      <c r="K203" s="10" t="s">
+        <v>1291</v>
+      </c>
+      <c r="L203" s="3">
+        <v>50.626206799999999</v>
+      </c>
+      <c r="M203" s="3">
+        <v>5.6625088000000003</v>
+      </c>
+      <c r="N203" s="3">
+        <v>2009</v>
+      </c>
+      <c r="O203" s="3">
+        <v>6</v>
+      </c>
+      <c r="Q203" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="V203" s="3">
+        <v>1</v>
+      </c>
+      <c r="W203" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="X203" s="3" t="s">
+        <v>1293</v>
+      </c>
+      <c r="Y203" s="3" t="s">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="204" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A204" s="3">
+        <v>203</v>
+      </c>
+      <c r="B204" s="3" t="s">
+        <v>1294</v>
+      </c>
+      <c r="C204" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D204" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="E204" s="3" t="s">
+        <v>1267</v>
+      </c>
+      <c r="F204" s="3" t="s">
+        <v>1295</v>
+      </c>
+      <c r="G204" s="3" t="s">
+        <v>1296</v>
+      </c>
+      <c r="H204" s="3" t="s">
+        <v>1297</v>
+      </c>
+      <c r="I204" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="K204" s="10" t="s">
+        <v>1299</v>
+      </c>
+      <c r="L204" s="3">
+        <v>50.84221385</v>
+      </c>
+      <c r="M204" s="3">
+        <v>4.3512390220279737</v>
+      </c>
+      <c r="N204" s="3">
+        <v>2012</v>
+      </c>
+      <c r="O204" s="3">
+        <v>9</v>
+      </c>
+      <c r="P204" s="3">
+        <v>11</v>
+      </c>
+      <c r="Q204" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="R204" s="3" t="s">
+        <v>1300</v>
+      </c>
+      <c r="S204" s="3" t="s">
+        <v>1301</v>
+      </c>
+      <c r="V204" s="3">
+        <v>1</v>
+      </c>
+      <c r="W204" s="3" t="s">
+        <v>1302</v>
+      </c>
+      <c r="X204" s="3" t="s">
+        <v>1303</v>
+      </c>
+      <c r="Y204" s="3" t="s">
+        <v>1304</v>
+      </c>
+    </row>
+    <row r="205" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A205" s="3">
+        <v>204</v>
+      </c>
+      <c r="B205" s="3" t="s">
+        <v>1305</v>
+      </c>
+      <c r="C205" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="D205" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="E205" s="3" t="s">
+        <v>1267</v>
+      </c>
+      <c r="F205" s="3" t="s">
+        <v>1295</v>
+      </c>
+      <c r="G205" s="3" t="s">
+        <v>1296</v>
+      </c>
+      <c r="H205" s="3" t="s">
+        <v>1306</v>
+      </c>
+      <c r="I205" s="3" t="s">
+        <v>1307</v>
+      </c>
+      <c r="K205" s="10" t="s">
+        <v>1299</v>
+      </c>
+      <c r="L205" s="3">
+        <v>50.813389999999998</v>
+      </c>
+      <c r="M205" s="3">
+        <v>4.3823100000000004</v>
+      </c>
+      <c r="N205" s="3">
+        <v>1979</v>
+      </c>
+      <c r="Q205" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="V205" s="3">
+        <v>1</v>
+      </c>
+      <c r="W205" s="3" t="s">
+        <v>1308</v>
+      </c>
+      <c r="X205" s="3" t="s">
+        <v>1309</v>
+      </c>
+      <c r="Y205" s="3" t="s">
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="206" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A206" s="3">
+        <v>205</v>
+      </c>
+      <c r="B206" s="3" t="s">
+        <v>1311</v>
+      </c>
+      <c r="C206" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D206" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="E206" s="3" t="s">
+        <v>1267</v>
+      </c>
+      <c r="F206" s="3" t="s">
+        <v>1312</v>
+      </c>
+      <c r="N206" s="3">
+        <v>2003</v>
+      </c>
+      <c r="O206" s="3">
+        <v>9</v>
+      </c>
+      <c r="Q206" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="R206" s="3" t="s">
+        <v>1313</v>
+      </c>
+      <c r="S206" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="V206" s="3">
+        <v>0</v>
+      </c>
+      <c r="W206" s="3" t="s">
+        <v>1314</v>
+      </c>
+      <c r="X206" s="3" t="s">
+        <v>1315</v>
+      </c>
+      <c r="Y206" s="3" t="s">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="207" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A207" s="3">
+        <v>206</v>
+      </c>
+      <c r="B207" s="3" t="s">
+        <v>1317</v>
+      </c>
+      <c r="C207" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D207" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="E207" s="3" t="s">
+        <v>1267</v>
+      </c>
+      <c r="F207" s="3" t="s">
+        <v>1295</v>
+      </c>
+      <c r="G207" s="3" t="s">
+        <v>1318</v>
+      </c>
+      <c r="K207" s="10" t="s">
+        <v>1319</v>
+      </c>
+      <c r="L207" s="3">
+        <v>50.873317900000004</v>
+      </c>
+      <c r="M207" s="3">
+        <v>4.4096169999999999</v>
+      </c>
+      <c r="N207" s="3">
+        <v>2007</v>
+      </c>
+      <c r="O207" s="3">
+        <v>9</v>
+      </c>
+      <c r="P207" s="3">
+        <v>15</v>
+      </c>
+      <c r="Q207" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="V207" s="3">
+        <v>1</v>
+      </c>
+      <c r="W207" s="3" t="s">
+        <v>1302</v>
+      </c>
+      <c r="X207" s="3" t="s">
+        <v>1320</v>
+      </c>
+      <c r="Y207" s="3" t="s">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="208" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A208" s="3">
+        <v>207</v>
+      </c>
+      <c r="B208" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="C208" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D208" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="E208" s="3" t="s">
+        <v>1267</v>
+      </c>
+      <c r="F208" s="3" t="s">
+        <v>1268</v>
+      </c>
+      <c r="G208" s="3" t="s">
+        <v>1269</v>
+      </c>
+      <c r="H208" s="3" t="s">
+        <v>1322</v>
+      </c>
+      <c r="K208" s="10" t="s">
+        <v>1323</v>
+      </c>
+      <c r="L208" s="3">
+        <v>50.681490500000002</v>
+      </c>
+      <c r="M208" s="3">
+        <v>5.5247631000000004</v>
+      </c>
+      <c r="N208" s="3">
+        <v>2007</v>
+      </c>
+      <c r="O208" s="3">
+        <v>2</v>
+      </c>
+      <c r="P208" s="3">
+        <v>18</v>
+      </c>
+      <c r="Q208" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="V208" s="3">
+        <v>1</v>
+      </c>
+      <c r="W208" s="3" t="s">
+        <v>1324</v>
+      </c>
+      <c r="X208" s="3" t="s">
+        <v>1325</v>
+      </c>
+      <c r="Y208" s="3" t="s">
+        <v>1326</v>
+      </c>
+    </row>
+    <row r="209" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A209" s="3">
+        <v>208</v>
+      </c>
+      <c r="B209" s="3" t="s">
+        <v>1317</v>
+      </c>
+      <c r="C209" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D209" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="E209" s="3" t="s">
+        <v>1267</v>
+      </c>
+      <c r="F209" s="3" t="s">
+        <v>1295</v>
+      </c>
+      <c r="G209" s="3" t="s">
+        <v>1318</v>
+      </c>
+      <c r="K209" s="10" t="s">
+        <v>1319</v>
+      </c>
+      <c r="L209" s="3">
+        <v>50.873317900000004</v>
+      </c>
+      <c r="M209" s="3">
+        <v>4.4096169999999999</v>
+      </c>
+      <c r="N209" s="3">
+        <v>2007</v>
+      </c>
+      <c r="O209" s="3">
+        <v>2</v>
+      </c>
+      <c r="P209" s="3">
+        <v>18</v>
+      </c>
+      <c r="Q209" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="V209" s="3">
+        <v>1</v>
+      </c>
+      <c r="W209" s="3" t="s">
+        <v>1302</v>
+      </c>
+      <c r="Y209" s="3" t="s">
+        <v>1326</v>
+      </c>
+    </row>
+    <row r="210" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A210" s="3">
+        <v>209</v>
+      </c>
+      <c r="B210" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="C210" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D210" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="E210" s="3" t="s">
+        <v>1267</v>
+      </c>
+      <c r="F210" s="3" t="s">
+        <v>1268</v>
+      </c>
+      <c r="G210" s="3" t="s">
+        <v>1327</v>
+      </c>
+      <c r="H210" s="3" t="s">
+        <v>1328</v>
+      </c>
+      <c r="I210" s="3" t="s">
+        <v>1329</v>
+      </c>
+      <c r="J210" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="K210" s="10" t="s">
+        <v>1331</v>
+      </c>
+      <c r="L210" s="3">
+        <v>50.4569647</v>
+      </c>
+      <c r="M210" s="3">
+        <v>4.0447142999999999</v>
+      </c>
+      <c r="N210" s="3">
+        <v>2007</v>
+      </c>
+      <c r="O210" s="3">
+        <v>2</v>
+      </c>
+      <c r="P210" s="3">
+        <v>18</v>
+      </c>
+      <c r="Q210" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="V210" s="3">
+        <v>1</v>
+      </c>
+      <c r="W210" s="3" t="s">
+        <v>1332</v>
+      </c>
+      <c r="X210" s="3" t="s">
+        <v>1333</v>
+      </c>
+      <c r="Y210" s="3" t="s">
+        <v>1326</v>
+      </c>
+    </row>
+    <row r="211" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A211" s="3">
+        <v>210</v>
+      </c>
+      <c r="B211" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="C211" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D211" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="E211" s="3" t="s">
+        <v>1267</v>
+      </c>
+      <c r="F211" s="3" t="s">
+        <v>1268</v>
+      </c>
+      <c r="G211" s="3" t="s">
+        <v>1327</v>
+      </c>
+      <c r="H211" s="3" t="s">
+        <v>1334</v>
+      </c>
+      <c r="I211" s="3" t="s">
+        <v>1335</v>
+      </c>
+      <c r="J211" s="3" t="s">
+        <v>1336</v>
+      </c>
+      <c r="K211" s="10" t="s">
+        <v>1337</v>
+      </c>
+      <c r="L211" s="3">
+        <v>50.420504899999997</v>
+      </c>
+      <c r="M211" s="3">
+        <v>4.2198108000000003</v>
+      </c>
+      <c r="N211" s="3">
+        <v>2007</v>
+      </c>
+      <c r="O211" s="3">
+        <v>2</v>
+      </c>
+      <c r="P211" s="3">
+        <v>18</v>
+      </c>
+      <c r="Q211" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="V211" s="3">
+        <v>1</v>
+      </c>
+      <c r="W211" s="3" t="s">
+        <v>1338</v>
+      </c>
+      <c r="X211" s="3" t="s">
+        <v>1339</v>
+      </c>
+      <c r="Y211" s="3" t="s">
+        <v>1326</v>
+      </c>
+    </row>
+    <row r="212" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A212" s="3">
+        <v>211</v>
+      </c>
+      <c r="B212" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="C212" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D212" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="E212" s="3" t="s">
+        <v>1267</v>
+      </c>
+      <c r="F212" s="3" t="s">
+        <v>1268</v>
+      </c>
+      <c r="G212" s="3" t="s">
+        <v>1327</v>
+      </c>
+      <c r="H212" s="3" t="s">
+        <v>1340</v>
+      </c>
+      <c r="I212" s="3" t="s">
+        <v>1341</v>
+      </c>
+      <c r="J212" s="3" t="s">
+        <v>1342</v>
+      </c>
+      <c r="K212" s="10" t="s">
+        <v>1343</v>
+      </c>
+      <c r="L212" s="3">
+        <v>50.458941899999999</v>
+      </c>
+      <c r="M212" s="3">
+        <v>4.3726770999999998</v>
+      </c>
+      <c r="N212" s="3">
+        <v>2007</v>
+      </c>
+      <c r="O212" s="3">
+        <v>2</v>
+      </c>
+      <c r="P212" s="3">
+        <v>18</v>
+      </c>
+      <c r="Q212" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="V212" s="3">
+        <v>1</v>
+      </c>
+      <c r="W212" s="3" t="s">
+        <v>1344</v>
+      </c>
+      <c r="X212" s="3" t="s">
+        <v>1345</v>
+      </c>
+      <c r="Y212" s="3" t="s">
+        <v>1326</v>
+      </c>
+    </row>
+    <row r="213" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A213" s="3">
+        <v>212</v>
+      </c>
+      <c r="B213" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="C213" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D213" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="E213" s="3" t="s">
+        <v>1267</v>
+      </c>
+      <c r="F213" s="3" t="s">
+        <v>1268</v>
+      </c>
+      <c r="G213" s="3" t="s">
+        <v>1327</v>
+      </c>
+      <c r="H213" s="3" t="s">
+        <v>1346</v>
+      </c>
+      <c r="I213" s="3" t="s">
+        <v>1347</v>
+      </c>
+      <c r="K213" s="10" t="s">
+        <v>1348</v>
+      </c>
+      <c r="L213" s="3">
+        <v>50.615337400000001</v>
+      </c>
+      <c r="M213" s="3">
+        <v>3.8030187</v>
+      </c>
+      <c r="N213" s="3">
+        <v>2007</v>
+      </c>
+      <c r="O213" s="3">
+        <v>2</v>
+      </c>
+      <c r="P213" s="3">
+        <v>18</v>
+      </c>
+      <c r="Q213" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="V213" s="3">
+        <v>1</v>
+      </c>
+      <c r="W213" s="3" t="s">
+        <v>1349</v>
+      </c>
+      <c r="X213" s="3" t="s">
+        <v>1350</v>
+      </c>
+      <c r="Y213" s="3" t="s">
+        <v>1326</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New features for #7, Mexico and Italy data
</commit_message>
<xml_diff>
--- a/a-place-for-salvador-allende/a_place_for_salvador_allende.xlsx
+++ b/a-place-for-salvador-allende/a_place_for_salvador_allende.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://onemsci-my.sharepoint.com/personal/glo_canonoy_msci_com/Documents/03 Training/datasets-of-interest/a-place-for-salvador-allende/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1701" documentId="11_FF6F299C653B866D72320E251CEDB2C4009A2F63" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA12BCC1-DDAF-4DBE-AE5B-B8CD9F9A39AA}"/>
+  <xr:revisionPtr revIDLastSave="1706" documentId="11_FF6F299C653B866D72320E251CEDB2C4009A2F63" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D35169A8-03D7-4772-B925-3E74A8D87E27}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2609" uniqueCount="1351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2985" uniqueCount="1545">
   <si>
     <t>id</t>
   </si>
@@ -4301,6 +4301,613 @@
   </si>
   <si>
     <t>https://goo.gl/maps/VcEeq2wFxMWqPRLy6</t>
+  </si>
+  <si>
+    <t>Monumento y Auditorio Salvador Allende, Centro Universitario de Ciencias Sociales y Humanidades (CUCSH) de la Universidad de Guadalajara</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Jalisco</t>
+  </si>
+  <si>
+    <t>Guadalajara</t>
+  </si>
+  <si>
+    <t>La Normal</t>
+  </si>
+  <si>
+    <t>Avenida de los Maestros</t>
+  </si>
+  <si>
+    <t>Centro Universitario de Ciencias Sociales y Humanidades - CUCSH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ser joven y no ser revolucionario es una contradicción hasta biológica
+02 - Dic. - 1972 
+Dr. Salvador Allende Gossens
+</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/c6ubJfwasMEYmCK26</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2007/02/18/43-universidad-de-guadalajara</t>
+  </si>
+  <si>
+    <t>Escuela Primaria Estatal Presidente Doctor Salvador Allende (30EPR0607D)</t>
+  </si>
+  <si>
+    <t>Veracruz</t>
+  </si>
+  <si>
+    <t>Acayucan</t>
+  </si>
+  <si>
+    <t>96000</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/peBkDFzzWwrSXJSk6</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2012/08/25/581-acayucan-mexico</t>
+  </si>
+  <si>
+    <t>Escuela Secundaria Diurna N° 165 "Presidente Salvador Allende"</t>
+  </si>
+  <si>
+    <t>Mexico City</t>
+  </si>
+  <si>
+    <t>Iztapalapa</t>
+  </si>
+  <si>
+    <t>Unidad Habitacional Vicente Guerrero</t>
+  </si>
+  <si>
+    <t>Avenida Antonio Díaz Soto y Gama</t>
+  </si>
+  <si>
+    <t>09200</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/459246832</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/mK1krWggB5gGsW256</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2012/06/21/569-iztapalapa-ciudad-de-mexico</t>
+  </si>
+  <si>
+    <t>Colonia Citlalli</t>
+  </si>
+  <si>
+    <t>09660</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/168080671</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/sGj5iUaL5QStRGF89</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2010/07/02/483-iztapalapa-mexico</t>
+  </si>
+  <si>
+    <t>State of Mexico</t>
+  </si>
+  <si>
+    <t>Nezahualcóyotl</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/620181654</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/CkEaoTpRBCBRG78s6</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2010/01/17/449-ciudad-nezahualcoyotl-mexico</t>
+  </si>
+  <si>
+    <t>Centro de Enseñanza Superior "Salvador Allende" A.C.</t>
+  </si>
+  <si>
+    <t>Tlaxcala</t>
+  </si>
+  <si>
+    <t>Municipio de Tlaxcala</t>
+  </si>
+  <si>
+    <t>Tlaxcala de Xicohténcatl</t>
+  </si>
+  <si>
+    <t>La Loma Xicohténcatl</t>
+  </si>
+  <si>
+    <t>Calle 15</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/95694303</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/kCUo9qqyyHBvMzPD8</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2009/07/04/369-tlaxcala-mexico</t>
+  </si>
+  <si>
+    <t>Instituto Salvador Allende</t>
+  </si>
+  <si>
+    <t>Puebla</t>
+  </si>
+  <si>
+    <t>Centro Histórico de Puebla</t>
+  </si>
+  <si>
+    <t>Avenida 11 Oriente</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/FNqT47S2Tvbzh32e6</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2008/05/10/188-puebla-y-tlaxcala-mexico</t>
+  </si>
+  <si>
+    <t>Escuela Preparatoria Particular Salvador Allende</t>
+  </si>
+  <si>
+    <t>Hidalgo</t>
+  </si>
+  <si>
+    <t>Tepeapulco</t>
+  </si>
+  <si>
+    <t>Ciudad Sahagún</t>
+  </si>
+  <si>
+    <t>43990</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2008/03/09/152-ciudad-sahagun-mexico</t>
+  </si>
+  <si>
+    <t>Avenida Domingo Muñoz Chimalpain</t>
+  </si>
+  <si>
+    <t>Compañero Presidente 
+Salvador Allende
+Inmolado por la causa de la Justicia Social
+Homenaje de los trabajadores del Complejo Industrial Sahagún
+25 de octubre 1973</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/node/5341423016</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2008/02/04/142-ciudad-sahagun-mexico</t>
+  </si>
+  <si>
+    <t>Nayarit</t>
+  </si>
+  <si>
+    <t>Municipio de Tepic</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/node/5983610898</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2007/09/22/105-un-pueblo-llamado-salvador-allende</t>
+  </si>
+  <si>
+    <t>Viale S. Allende</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>Tuscany</t>
+  </si>
+  <si>
+    <t>Livorno</t>
+  </si>
+  <si>
+    <t>Cecina</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/680086127</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/ZDLRp15ufPPzQAah8</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2012/11/04/595-cecina-italia</t>
+  </si>
+  <si>
+    <t>Centro Salvador Allende</t>
+  </si>
+  <si>
+    <t>Liguria</t>
+  </si>
+  <si>
+    <t>La Spezia</t>
+  </si>
+  <si>
+    <t>Follo</t>
+  </si>
+  <si>
+    <t>Porta Rocca</t>
+  </si>
+  <si>
+    <t>19100</t>
+  </si>
+  <si>
+    <t>Comune della Spezia
+Salvador Allende - 11 settembre 1973
+"La storia è nostra e la fanno i popoli"
+La Spezia 1 settembre 2003
+Salvador Allende 1908 - 1973</t>
+  </si>
+  <si>
+    <t>it</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/205843492</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2012/09/01/573-la-spezia-italia</t>
+  </si>
+  <si>
+    <t>Memorial plate to Salvador Allende and victims of the Chilean dictatorship at Viale 11 Settembre 1973</t>
+  </si>
+  <si>
+    <t>Florence</t>
+  </si>
+  <si>
+    <t>Lastra a Signa</t>
+  </si>
+  <si>
+    <t>Stagno</t>
+  </si>
+  <si>
+    <t>Via 11 settembre 1973</t>
+  </si>
+  <si>
+    <t>Viale 11 Settembre 1973
+In memoria di Salvador Allende  e di tutte le vittime della dittatura cilena "1973 - 1989" di Pinochet
+Lastra a Signa 27.1.2004 - 
+Comune Di Lastra A Signa - Comitato Dei Lavoratori  Cileni Esiliati</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/72568206</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/5Jx7Da4qM5rJ1MBY6</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2012/06/27/574-lastra-a-signa-italia</t>
+  </si>
+  <si>
+    <t>Via Salvatore Allende</t>
+  </si>
+  <si>
+    <t>Lazio</t>
+  </si>
+  <si>
+    <t>Viterbo</t>
+  </si>
+  <si>
+    <t>Bolsena</t>
+  </si>
+  <si>
+    <t>01023</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/LQATSSSkfs7LbeWc6</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2011/12/10/540-bolsena-italia</t>
+  </si>
+  <si>
+    <t>Largo Salvador Allende</t>
+  </si>
+  <si>
+    <t>Marche</t>
+  </si>
+  <si>
+    <t>Ancona</t>
+  </si>
+  <si>
+    <t>Jesi</t>
+  </si>
+  <si>
+    <t>Santiago 11 Settembre 1973
+Il mio sacrificio
+non sarà vano:
+Viva il Cile
+Viva il popolo cileno
+Il presidente Salvador Allende, martire del socialismo e della democrazia.
+La citta di Jesi
+11 Settembre 1983</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/nMLFVFk6e9GGEXce7</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2011/02/22/513-jesi-italia</t>
+  </si>
+  <si>
+    <t>Via Salvador Allende</t>
+  </si>
+  <si>
+    <t>Calabria</t>
+  </si>
+  <si>
+    <t>Cosenza</t>
+  </si>
+  <si>
+    <t>Rende</t>
+  </si>
+  <si>
+    <t>Roges</t>
+  </si>
+  <si>
+    <t>87036</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/31143754</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/7DaQpbA71yzn75fTA</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2010/11/15/504-cosenza-italia</t>
+  </si>
+  <si>
+    <t>Lombardy</t>
+  </si>
+  <si>
+    <t>Milan</t>
+  </si>
+  <si>
+    <t>Lacchiarella</t>
+  </si>
+  <si>
+    <t>Mettone</t>
+  </si>
+  <si>
+    <t>Cascina Fiorano</t>
+  </si>
+  <si>
+    <t>20084</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/41993630</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/mc9ogqgbZMBXeiGM7</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2010/07/28/465-lacchiarella-italia</t>
+  </si>
+  <si>
+    <t>Albairate</t>
+  </si>
+  <si>
+    <t>20081</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/43809646</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/mEUVDTZTdKZafbjZ6</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2010/04/01/460-albairate-italia</t>
+  </si>
+  <si>
+    <t>San Donato Milanese</t>
+  </si>
+  <si>
+    <t>Poasco</t>
+  </si>
+  <si>
+    <t>Sorigherio</t>
+  </si>
+  <si>
+    <t>20097</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/194280635</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/eCwuhSWRUz5LVAa69</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2010/01/23/467-san-donato-milanese-italia</t>
+  </si>
+  <si>
+    <t>Istituto S. Allende - P. Custodi [muzzu]</t>
+  </si>
+  <si>
+    <t>Chiesa Rossa</t>
+  </si>
+  <si>
+    <t>Stadera</t>
+  </si>
+  <si>
+    <t>Bicentenario della proclamazione dei Diritti dell'Uomo 1789 - 1989
+Santiago del Cile 11 Settembre 1973
+Salvador Allende
+Martire della libertá
+Esempio altamente significativo di una generosa dedizione alla causa del progresso civile e sociale del proprio paese</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/XCgMQiBjuqHCoL8JA</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2009/11/19/439-milan-italia</t>
+  </si>
+  <si>
+    <t>Campania</t>
+  </si>
+  <si>
+    <t>Salerno</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/288706835</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/BqcTt6MEEHRMWTEC6</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2007/02/18/26-italia</t>
+  </si>
+  <si>
+    <t>Campi Bisenzio</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/604326920</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/jufuk3wnYovPD2Kp9</t>
+  </si>
+  <si>
+    <t>Baronissi</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/292875519</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/dnQAZzZncCcVqMqT7</t>
+  </si>
+  <si>
+    <t>Ardenza</t>
+  </si>
+  <si>
+    <t>57128</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/29071177</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/VS6eFsnzkWtsZzWV8</t>
+  </si>
+  <si>
+    <t>Arese</t>
+  </si>
+  <si>
+    <t>Valera</t>
+  </si>
+  <si>
+    <t>Supresada</t>
+  </si>
+  <si>
+    <t>20044</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/1086753669</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/B1ZEdKxoWVUpD7dQ9</t>
+  </si>
+  <si>
+    <t>Genoa</t>
+  </si>
+  <si>
+    <t>Media Val Bisagno</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/732154120</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/rex2GgaD8acNGNzg9</t>
+  </si>
+  <si>
+    <t>Emilia-Romagna</t>
+  </si>
+  <si>
+    <t>Reggio nell'Emilia</t>
+  </si>
+  <si>
+    <t>Colline Matildiche</t>
+  </si>
+  <si>
+    <t>Quattro Castella</t>
+  </si>
+  <si>
+    <t>Montecavolo</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/86174113</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/FsGojBG2TzzyMMfs9</t>
+  </si>
+  <si>
+    <t>Mantua</t>
+  </si>
+  <si>
+    <t>Quistello</t>
+  </si>
+  <si>
+    <t>Conventino</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/293526101</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/CTUHLuS4h3fK1Y3E7</t>
+  </si>
+  <si>
+    <t>Piazza Salvador Allende</t>
+  </si>
+  <si>
+    <t>Abruzzo</t>
+  </si>
+  <si>
+    <t>Pescara</t>
+  </si>
+  <si>
+    <t>Rancitelli</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/relation/13468348</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/Gvw49FS2ZP4LGXJy6</t>
+  </si>
+  <si>
+    <t>Forlì-Cesena</t>
+  </si>
+  <si>
+    <t>Bagno di Romagna</t>
+  </si>
+  <si>
+    <t>San Piero in Bagno</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/336150404</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/hBmqibUFgsmJdPHm6</t>
+  </si>
+  <si>
+    <t>Arenzano</t>
+  </si>
+  <si>
+    <t>Borghetto</t>
+  </si>
+  <si>
+    <t>Crocetta</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/87321538</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/cpr44t88iWfcRxSz5</t>
   </si>
 </sst>
 </file>
@@ -4635,13 +5242,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AO213"/>
+  <dimension ref="A1:AO244"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B195" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B236" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A214" sqref="A214"/>
+      <selection pane="bottomRight" activeCell="A245" sqref="A245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -17893,6 +18500,1841 @@
       </c>
       <c r="Y213" s="3" t="s">
         <v>1326</v>
+      </c>
+    </row>
+    <row r="214" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A214" s="3">
+        <v>213</v>
+      </c>
+      <c r="B214" s="3" t="s">
+        <v>1351</v>
+      </c>
+      <c r="C214" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D214" s="3" t="s">
+        <v>851</v>
+      </c>
+      <c r="E214" s="3" t="s">
+        <v>1352</v>
+      </c>
+      <c r="F214" s="3" t="s">
+        <v>1353</v>
+      </c>
+      <c r="G214" s="3" t="s">
+        <v>1354</v>
+      </c>
+      <c r="H214" s="3" t="s">
+        <v>1355</v>
+      </c>
+      <c r="I214" s="3" t="s">
+        <v>1356</v>
+      </c>
+      <c r="J214" s="3" t="s">
+        <v>1357</v>
+      </c>
+      <c r="K214" s="10">
+        <v>44260</v>
+      </c>
+      <c r="L214" s="3">
+        <v>20.694000854896998</v>
+      </c>
+      <c r="M214" s="3">
+        <v>-103.349162153896</v>
+      </c>
+      <c r="N214" s="3">
+        <v>2007</v>
+      </c>
+      <c r="O214" s="3">
+        <v>2</v>
+      </c>
+      <c r="P214" s="3">
+        <v>18</v>
+      </c>
+      <c r="Q214" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="R214" s="3" t="s">
+        <v>1358</v>
+      </c>
+      <c r="S214" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="V214" s="3">
+        <v>1</v>
+      </c>
+      <c r="X214" s="3" t="s">
+        <v>1359</v>
+      </c>
+      <c r="Y214" s="3" t="s">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="215" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A215" s="3">
+        <v>214</v>
+      </c>
+      <c r="B215" s="3" t="s">
+        <v>1361</v>
+      </c>
+      <c r="C215" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D215" s="3" t="s">
+        <v>851</v>
+      </c>
+      <c r="E215" s="3" t="s">
+        <v>1352</v>
+      </c>
+      <c r="F215" s="3" t="s">
+        <v>1362</v>
+      </c>
+      <c r="G215" s="3" t="s">
+        <v>1363</v>
+      </c>
+      <c r="K215" s="10" t="s">
+        <v>1364</v>
+      </c>
+      <c r="L215" s="3">
+        <v>17.951541403234199</v>
+      </c>
+      <c r="M215" s="3">
+        <v>-94.924099182931201</v>
+      </c>
+      <c r="N215" s="3">
+        <v>2012</v>
+      </c>
+      <c r="O215" s="3">
+        <v>7</v>
+      </c>
+      <c r="Q215" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="V215" s="3">
+        <v>1</v>
+      </c>
+      <c r="X215" s="3" t="s">
+        <v>1365</v>
+      </c>
+      <c r="Y215" s="3" t="s">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="216" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A216" s="3">
+        <v>215</v>
+      </c>
+      <c r="B216" s="3" t="s">
+        <v>1367</v>
+      </c>
+      <c r="C216" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D216" s="3" t="s">
+        <v>851</v>
+      </c>
+      <c r="E216" s="3" t="s">
+        <v>1352</v>
+      </c>
+      <c r="F216" s="3" t="s">
+        <v>1368</v>
+      </c>
+      <c r="G216" s="3" t="s">
+        <v>1369</v>
+      </c>
+      <c r="H216" s="3" t="s">
+        <v>1370</v>
+      </c>
+      <c r="I216" s="3" t="s">
+        <v>1371</v>
+      </c>
+      <c r="K216" s="10" t="s">
+        <v>1372</v>
+      </c>
+      <c r="L216" s="3">
+        <v>19.358027393529301</v>
+      </c>
+      <c r="M216" s="3">
+        <v>-99.049278253635293</v>
+      </c>
+      <c r="N216" s="3">
+        <v>2008</v>
+      </c>
+      <c r="O216" s="3">
+        <v>12</v>
+      </c>
+      <c r="Q216" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="V216" s="3">
+        <v>1</v>
+      </c>
+      <c r="W216" s="3" t="s">
+        <v>1373</v>
+      </c>
+      <c r="X216" s="3" t="s">
+        <v>1374</v>
+      </c>
+      <c r="Y216" s="3" t="s">
+        <v>1375</v>
+      </c>
+    </row>
+    <row r="217" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A217" s="3">
+        <v>216</v>
+      </c>
+      <c r="B217" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C217" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D217" s="3" t="s">
+        <v>851</v>
+      </c>
+      <c r="E217" s="3" t="s">
+        <v>1352</v>
+      </c>
+      <c r="F217" s="3" t="s">
+        <v>1368</v>
+      </c>
+      <c r="G217" s="3" t="s">
+        <v>1369</v>
+      </c>
+      <c r="H217" s="3" t="s">
+        <v>1376</v>
+      </c>
+      <c r="K217" s="10" t="s">
+        <v>1377</v>
+      </c>
+      <c r="L217" s="3">
+        <v>19.342850567880699</v>
+      </c>
+      <c r="M217" s="3">
+        <v>-99.025879505879601</v>
+      </c>
+      <c r="N217" s="3">
+        <v>2009</v>
+      </c>
+      <c r="O217" s="3">
+        <v>9</v>
+      </c>
+      <c r="Q217" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="V217" s="3">
+        <v>1</v>
+      </c>
+      <c r="W217" s="3" t="s">
+        <v>1378</v>
+      </c>
+      <c r="X217" s="3" t="s">
+        <v>1379</v>
+      </c>
+      <c r="Y217" s="3" t="s">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="218" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A218" s="3">
+        <v>217</v>
+      </c>
+      <c r="B218" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C218" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D218" s="3" t="s">
+        <v>851</v>
+      </c>
+      <c r="E218" s="3" t="s">
+        <v>1352</v>
+      </c>
+      <c r="F218" s="3" t="s">
+        <v>1381</v>
+      </c>
+      <c r="G218" s="3" t="s">
+        <v>1382</v>
+      </c>
+      <c r="K218" s="10">
+        <v>57200</v>
+      </c>
+      <c r="L218" s="3">
+        <v>19.4389228278818</v>
+      </c>
+      <c r="M218" s="3">
+        <v>-99.047545341022399</v>
+      </c>
+      <c r="N218" s="3">
+        <v>2009</v>
+      </c>
+      <c r="O218" s="3">
+        <v>7</v>
+      </c>
+      <c r="Q218" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="V218" s="3">
+        <v>1</v>
+      </c>
+      <c r="W218" s="3" t="s">
+        <v>1383</v>
+      </c>
+      <c r="X218" s="3" t="s">
+        <v>1384</v>
+      </c>
+      <c r="Y218" s="3" t="s">
+        <v>1385</v>
+      </c>
+    </row>
+    <row r="219" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A219" s="3">
+        <v>218</v>
+      </c>
+      <c r="B219" s="3" t="s">
+        <v>1386</v>
+      </c>
+      <c r="C219" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D219" s="3" t="s">
+        <v>851</v>
+      </c>
+      <c r="E219" s="3" t="s">
+        <v>1352</v>
+      </c>
+      <c r="F219" s="3" t="s">
+        <v>1387</v>
+      </c>
+      <c r="G219" s="3" t="s">
+        <v>1388</v>
+      </c>
+      <c r="H219" s="3" t="s">
+        <v>1389</v>
+      </c>
+      <c r="I219" s="3" t="s">
+        <v>1390</v>
+      </c>
+      <c r="J219" s="3" t="s">
+        <v>1391</v>
+      </c>
+      <c r="K219" s="10">
+        <v>90070</v>
+      </c>
+      <c r="L219" s="3">
+        <v>19.310253516839602</v>
+      </c>
+      <c r="M219" s="3">
+        <v>-98.242347266063604</v>
+      </c>
+      <c r="N219" s="3">
+        <v>2009</v>
+      </c>
+      <c r="O219" s="3">
+        <v>7</v>
+      </c>
+      <c r="P219" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q219" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="V219" s="3">
+        <v>1</v>
+      </c>
+      <c r="W219" s="3" t="s">
+        <v>1392</v>
+      </c>
+      <c r="X219" s="3" t="s">
+        <v>1393</v>
+      </c>
+      <c r="Y219" s="3" t="s">
+        <v>1394</v>
+      </c>
+    </row>
+    <row r="220" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A220" s="3">
+        <v>219</v>
+      </c>
+      <c r="B220" s="3" t="s">
+        <v>1395</v>
+      </c>
+      <c r="C220" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D220" s="3" t="s">
+        <v>851</v>
+      </c>
+      <c r="E220" s="3" t="s">
+        <v>1352</v>
+      </c>
+      <c r="F220" s="3" t="s">
+        <v>1396</v>
+      </c>
+      <c r="G220" s="3" t="s">
+        <v>1397</v>
+      </c>
+      <c r="H220" s="3" t="s">
+        <v>1398</v>
+      </c>
+      <c r="K220" s="10">
+        <v>72000</v>
+      </c>
+      <c r="L220" s="3">
+        <v>19.0399756505612</v>
+      </c>
+      <c r="M220" s="3">
+        <v>-98.199669116586904</v>
+      </c>
+      <c r="N220" s="3">
+        <v>2008</v>
+      </c>
+      <c r="O220" s="3">
+        <v>5</v>
+      </c>
+      <c r="P220" s="3">
+        <v>10</v>
+      </c>
+      <c r="Q220" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="V220" s="3">
+        <v>1</v>
+      </c>
+      <c r="X220" s="3" t="s">
+        <v>1399</v>
+      </c>
+      <c r="Y220" s="3" t="s">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="221" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A221" s="3">
+        <v>220</v>
+      </c>
+      <c r="B221" s="3" t="s">
+        <v>1401</v>
+      </c>
+      <c r="C221" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D221" s="3" t="s">
+        <v>851</v>
+      </c>
+      <c r="E221" s="3" t="s">
+        <v>1352</v>
+      </c>
+      <c r="F221" s="3" t="s">
+        <v>1402</v>
+      </c>
+      <c r="G221" s="3" t="s">
+        <v>1403</v>
+      </c>
+      <c r="H221" s="3" t="s">
+        <v>1404</v>
+      </c>
+      <c r="K221" s="10" t="s">
+        <v>1405</v>
+      </c>
+      <c r="N221" s="3">
+        <v>1973</v>
+      </c>
+      <c r="Q221" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="V221" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y221" s="3" t="s">
+        <v>1406</v>
+      </c>
+    </row>
+    <row r="222" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A222" s="3">
+        <v>221</v>
+      </c>
+      <c r="B222" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C222" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D222" s="3" t="s">
+        <v>851</v>
+      </c>
+      <c r="E222" s="3" t="s">
+        <v>1352</v>
+      </c>
+      <c r="F222" s="3" t="s">
+        <v>1402</v>
+      </c>
+      <c r="G222" s="3" t="s">
+        <v>1403</v>
+      </c>
+      <c r="H222" s="3" t="s">
+        <v>1404</v>
+      </c>
+      <c r="I222" s="3" t="s">
+        <v>1407</v>
+      </c>
+      <c r="K222" s="10" t="s">
+        <v>1405</v>
+      </c>
+      <c r="L222" s="3">
+        <v>19.771550000000001</v>
+      </c>
+      <c r="M222" s="3">
+        <v>-98.578109999999995</v>
+      </c>
+      <c r="N222" s="3">
+        <v>1973</v>
+      </c>
+      <c r="O222" s="3">
+        <v>10</v>
+      </c>
+      <c r="P222" s="3">
+        <v>25</v>
+      </c>
+      <c r="Q222" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="R222" s="3" t="s">
+        <v>1408</v>
+      </c>
+      <c r="S222" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="V222" s="3">
+        <v>1</v>
+      </c>
+      <c r="W222" s="3" t="s">
+        <v>1409</v>
+      </c>
+      <c r="Y222" s="3" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="223" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A223" s="3">
+        <v>222</v>
+      </c>
+      <c r="B223" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C223" s="3" t="s">
+        <v>802</v>
+      </c>
+      <c r="D223" s="3" t="s">
+        <v>851</v>
+      </c>
+      <c r="E223" s="3" t="s">
+        <v>1352</v>
+      </c>
+      <c r="F223" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G223" s="3" t="s">
+        <v>1412</v>
+      </c>
+      <c r="K223" s="10">
+        <v>63751</v>
+      </c>
+      <c r="L223" s="3">
+        <v>21.69528</v>
+      </c>
+      <c r="M223" s="3">
+        <v>-104.90225</v>
+      </c>
+      <c r="N223" s="3">
+        <v>1984</v>
+      </c>
+      <c r="Q223" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="V223" s="3">
+        <v>1</v>
+      </c>
+      <c r="W223" s="3" t="s">
+        <v>1413</v>
+      </c>
+      <c r="Y223" s="3" t="s">
+        <v>1414</v>
+      </c>
+    </row>
+    <row r="224" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A224" s="3">
+        <v>223</v>
+      </c>
+      <c r="B224" s="3" t="s">
+        <v>1415</v>
+      </c>
+      <c r="C224" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D224" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="E224" s="3" t="s">
+        <v>1416</v>
+      </c>
+      <c r="F224" s="3" t="s">
+        <v>1417</v>
+      </c>
+      <c r="G224" s="3" t="s">
+        <v>1418</v>
+      </c>
+      <c r="H224" s="3" t="s">
+        <v>1419</v>
+      </c>
+      <c r="K224" s="10">
+        <v>57023</v>
+      </c>
+      <c r="L224" s="3">
+        <v>43.311218108065702</v>
+      </c>
+      <c r="M224" s="3">
+        <v>10.5320137144572</v>
+      </c>
+      <c r="N224" s="3">
+        <v>2012</v>
+      </c>
+      <c r="O224" s="3">
+        <v>11</v>
+      </c>
+      <c r="P224" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q224" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="V224" s="3">
+        <v>1</v>
+      </c>
+      <c r="W224" s="3" t="s">
+        <v>1420</v>
+      </c>
+      <c r="X224" s="3" t="s">
+        <v>1421</v>
+      </c>
+      <c r="Y224" s="3" t="s">
+        <v>1422</v>
+      </c>
+    </row>
+    <row r="225" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A225" s="3">
+        <v>224</v>
+      </c>
+      <c r="B225" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="C225" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="D225" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="E225" s="3" t="s">
+        <v>1416</v>
+      </c>
+      <c r="F225" s="3" t="s">
+        <v>1424</v>
+      </c>
+      <c r="G225" s="3" t="s">
+        <v>1425</v>
+      </c>
+      <c r="H225" s="3" t="s">
+        <v>1426</v>
+      </c>
+      <c r="I225" s="3" t="s">
+        <v>1425</v>
+      </c>
+      <c r="J225" s="3" t="s">
+        <v>1427</v>
+      </c>
+      <c r="K225" s="10" t="s">
+        <v>1428</v>
+      </c>
+      <c r="L225" s="3">
+        <v>44.10282505</v>
+      </c>
+      <c r="M225" s="3">
+        <v>9.8241184374151622</v>
+      </c>
+      <c r="N225" s="3">
+        <v>2003</v>
+      </c>
+      <c r="O225" s="3">
+        <v>9</v>
+      </c>
+      <c r="P225" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q225" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="R225" s="3" t="s">
+        <v>1429</v>
+      </c>
+      <c r="S225" s="3" t="s">
+        <v>1430</v>
+      </c>
+      <c r="V225" s="3">
+        <v>1</v>
+      </c>
+      <c r="W225" s="3" t="s">
+        <v>1431</v>
+      </c>
+      <c r="Y225" s="3" t="s">
+        <v>1432</v>
+      </c>
+    </row>
+    <row r="226" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A226" s="3">
+        <v>225</v>
+      </c>
+      <c r="B226" s="3" t="s">
+        <v>1433</v>
+      </c>
+      <c r="C226" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D226" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="E226" s="3" t="s">
+        <v>1416</v>
+      </c>
+      <c r="F226" s="3" t="s">
+        <v>1417</v>
+      </c>
+      <c r="G226" s="3" t="s">
+        <v>1434</v>
+      </c>
+      <c r="H226" s="3" t="s">
+        <v>1435</v>
+      </c>
+      <c r="I226" s="3" t="s">
+        <v>1436</v>
+      </c>
+      <c r="J226" s="3" t="s">
+        <v>1437</v>
+      </c>
+      <c r="K226" s="10">
+        <v>50058</v>
+      </c>
+      <c r="L226" s="3">
+        <v>43.774190238583202</v>
+      </c>
+      <c r="M226" s="3">
+        <v>11.118669043316601</v>
+      </c>
+      <c r="N226" s="3">
+        <v>2004</v>
+      </c>
+      <c r="O226" s="3">
+        <v>1</v>
+      </c>
+      <c r="P226" s="3">
+        <v>27</v>
+      </c>
+      <c r="Q226" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="R226" s="3" t="s">
+        <v>1438</v>
+      </c>
+      <c r="S226" s="3" t="s">
+        <v>1430</v>
+      </c>
+      <c r="V226" s="3">
+        <v>1</v>
+      </c>
+      <c r="W226" s="3" t="s">
+        <v>1439</v>
+      </c>
+      <c r="X226" s="3" t="s">
+        <v>1440</v>
+      </c>
+      <c r="Y226" s="3" t="s">
+        <v>1441</v>
+      </c>
+    </row>
+    <row r="227" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A227" s="3">
+        <v>226</v>
+      </c>
+      <c r="B227" s="3" t="s">
+        <v>1442</v>
+      </c>
+      <c r="C227" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D227" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="E227" s="3" t="s">
+        <v>1416</v>
+      </c>
+      <c r="F227" s="3" t="s">
+        <v>1443</v>
+      </c>
+      <c r="G227" s="3" t="s">
+        <v>1444</v>
+      </c>
+      <c r="H227" s="3" t="s">
+        <v>1445</v>
+      </c>
+      <c r="K227" s="10" t="s">
+        <v>1446</v>
+      </c>
+      <c r="L227" s="3">
+        <v>42.647382943214801</v>
+      </c>
+      <c r="M227" s="3">
+        <v>11.9785530528076</v>
+      </c>
+      <c r="N227" s="3">
+        <v>2011</v>
+      </c>
+      <c r="O227" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q227" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="V227" s="3">
+        <v>1</v>
+      </c>
+      <c r="X227" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="Y227" s="3" t="s">
+        <v>1448</v>
+      </c>
+    </row>
+    <row r="228" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A228" s="3">
+        <v>227</v>
+      </c>
+      <c r="B228" s="3" t="s">
+        <v>1449</v>
+      </c>
+      <c r="C228" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D228" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="E228" s="3" t="s">
+        <v>1416</v>
+      </c>
+      <c r="F228" s="3" t="s">
+        <v>1450</v>
+      </c>
+      <c r="G228" s="3" t="s">
+        <v>1451</v>
+      </c>
+      <c r="H228" s="3" t="s">
+        <v>1452</v>
+      </c>
+      <c r="L228" s="3">
+        <v>43.516691667878298</v>
+      </c>
+      <c r="M228" s="3">
+        <v>13.228280608917499</v>
+      </c>
+      <c r="N228" s="3">
+        <v>1983</v>
+      </c>
+      <c r="O228" s="3">
+        <v>9</v>
+      </c>
+      <c r="P228" s="3">
+        <v>11</v>
+      </c>
+      <c r="Q228" s="3" t="s">
+        <v>686</v>
+      </c>
+      <c r="R228" s="3" t="s">
+        <v>1453</v>
+      </c>
+      <c r="S228" s="3" t="s">
+        <v>1430</v>
+      </c>
+      <c r="V228" s="3">
+        <v>1</v>
+      </c>
+      <c r="X228" s="3" t="s">
+        <v>1454</v>
+      </c>
+      <c r="Y228" s="3" t="s">
+        <v>1455</v>
+      </c>
+    </row>
+    <row r="229" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A229" s="3">
+        <v>228</v>
+      </c>
+      <c r="B229" s="3" t="s">
+        <v>1456</v>
+      </c>
+      <c r="C229" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D229" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="E229" s="3" t="s">
+        <v>1416</v>
+      </c>
+      <c r="F229" s="3" t="s">
+        <v>1457</v>
+      </c>
+      <c r="G229" s="3" t="s">
+        <v>1458</v>
+      </c>
+      <c r="H229" s="3" t="s">
+        <v>1459</v>
+      </c>
+      <c r="I229" s="3" t="s">
+        <v>1460</v>
+      </c>
+      <c r="K229" s="10" t="s">
+        <v>1461</v>
+      </c>
+      <c r="L229" s="3">
+        <v>39.330146900000003</v>
+      </c>
+      <c r="M229" s="3">
+        <v>16.242617500000001</v>
+      </c>
+      <c r="N229" s="3">
+        <v>2009</v>
+      </c>
+      <c r="O229" s="3">
+        <v>8</v>
+      </c>
+      <c r="Q229" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="V229" s="3">
+        <v>1</v>
+      </c>
+      <c r="W229" s="3" t="s">
+        <v>1462</v>
+      </c>
+      <c r="X229" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="Y229" s="3" t="s">
+        <v>1464</v>
+      </c>
+    </row>
+    <row r="230" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A230" s="3">
+        <v>229</v>
+      </c>
+      <c r="B230" s="3" t="s">
+        <v>1456</v>
+      </c>
+      <c r="C230" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D230" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="E230" s="3" t="s">
+        <v>1416</v>
+      </c>
+      <c r="F230" s="3" t="s">
+        <v>1465</v>
+      </c>
+      <c r="G230" s="3" t="s">
+        <v>1466</v>
+      </c>
+      <c r="H230" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="I230" s="3" t="s">
+        <v>1468</v>
+      </c>
+      <c r="J230" s="3" t="s">
+        <v>1469</v>
+      </c>
+      <c r="K230" s="10" t="s">
+        <v>1470</v>
+      </c>
+      <c r="L230" s="3">
+        <v>45.324244399999998</v>
+      </c>
+      <c r="M230" s="3">
+        <v>9.1460881999999994</v>
+      </c>
+      <c r="N230" s="3">
+        <v>2008</v>
+      </c>
+      <c r="O230" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q230" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="V230" s="3">
+        <v>1</v>
+      </c>
+      <c r="W230" s="3" t="s">
+        <v>1471</v>
+      </c>
+      <c r="X230" s="3" t="s">
+        <v>1472</v>
+      </c>
+      <c r="Y230" s="3" t="s">
+        <v>1473</v>
+      </c>
+    </row>
+    <row r="231" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A231" s="3">
+        <v>230</v>
+      </c>
+      <c r="B231" s="3" t="s">
+        <v>1456</v>
+      </c>
+      <c r="C231" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D231" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="E231" s="3" t="s">
+        <v>1416</v>
+      </c>
+      <c r="F231" s="3" t="s">
+        <v>1465</v>
+      </c>
+      <c r="G231" s="3" t="s">
+        <v>1466</v>
+      </c>
+      <c r="H231" s="3" t="s">
+        <v>1474</v>
+      </c>
+      <c r="K231" s="10" t="s">
+        <v>1475</v>
+      </c>
+      <c r="L231" s="3">
+        <v>45.416547000000001</v>
+      </c>
+      <c r="M231" s="3">
+        <v>8.9368069000000006</v>
+      </c>
+      <c r="N231" s="3">
+        <v>2008</v>
+      </c>
+      <c r="O231" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q231" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="V231" s="3">
+        <v>1</v>
+      </c>
+      <c r="W231" s="3" t="s">
+        <v>1476</v>
+      </c>
+      <c r="X231" s="3" t="s">
+        <v>1477</v>
+      </c>
+      <c r="Y231" s="3" t="s">
+        <v>1478</v>
+      </c>
+    </row>
+    <row r="232" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A232" s="3">
+        <v>231</v>
+      </c>
+      <c r="B232" s="3" t="s">
+        <v>1456</v>
+      </c>
+      <c r="C232" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D232" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="E232" s="3" t="s">
+        <v>1416</v>
+      </c>
+      <c r="F232" s="3" t="s">
+        <v>1465</v>
+      </c>
+      <c r="G232" s="3" t="s">
+        <v>1466</v>
+      </c>
+      <c r="H232" s="3" t="s">
+        <v>1479</v>
+      </c>
+      <c r="I232" s="3" t="s">
+        <v>1480</v>
+      </c>
+      <c r="J232" s="3" t="s">
+        <v>1481</v>
+      </c>
+      <c r="K232" s="10" t="s">
+        <v>1482</v>
+      </c>
+      <c r="L232" s="3">
+        <v>45.404805500000002</v>
+      </c>
+      <c r="M232" s="3">
+        <v>9.2313098</v>
+      </c>
+      <c r="N232" s="3">
+        <v>2008</v>
+      </c>
+      <c r="O232" s="3">
+        <v>6</v>
+      </c>
+      <c r="Q232" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="V232" s="3">
+        <v>1</v>
+      </c>
+      <c r="W232" s="3" t="s">
+        <v>1483</v>
+      </c>
+      <c r="X232" s="3" t="s">
+        <v>1484</v>
+      </c>
+      <c r="Y232" s="3" t="s">
+        <v>1485</v>
+      </c>
+    </row>
+    <row r="233" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A233" s="3">
+        <v>232</v>
+      </c>
+      <c r="B233" s="3" t="s">
+        <v>1486</v>
+      </c>
+      <c r="C233" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D233" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="E233" s="3" t="s">
+        <v>1416</v>
+      </c>
+      <c r="F233" s="3" t="s">
+        <v>1465</v>
+      </c>
+      <c r="G233" s="3" t="s">
+        <v>1466</v>
+      </c>
+      <c r="H233" s="3" t="s">
+        <v>1487</v>
+      </c>
+      <c r="I233" s="3" t="s">
+        <v>1488</v>
+      </c>
+      <c r="K233" s="10">
+        <v>20141</v>
+      </c>
+      <c r="L233" s="3">
+        <v>45.4293940133863</v>
+      </c>
+      <c r="M233" s="3">
+        <v>9.1798862076386403</v>
+      </c>
+      <c r="N233" s="3">
+        <v>1989</v>
+      </c>
+      <c r="Q233" s="3" t="s">
+        <v>686</v>
+      </c>
+      <c r="R233" s="3" t="s">
+        <v>1489</v>
+      </c>
+      <c r="S233" s="3" t="s">
+        <v>1430</v>
+      </c>
+      <c r="V233" s="3">
+        <v>1</v>
+      </c>
+      <c r="X233" s="3" t="s">
+        <v>1490</v>
+      </c>
+      <c r="Y233" s="3" t="s">
+        <v>1491</v>
+      </c>
+    </row>
+    <row r="234" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A234" s="3">
+        <v>233</v>
+      </c>
+      <c r="B234" s="3" t="s">
+        <v>1456</v>
+      </c>
+      <c r="C234" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D234" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="E234" s="3" t="s">
+        <v>1416</v>
+      </c>
+      <c r="F234" s="3" t="s">
+        <v>1492</v>
+      </c>
+      <c r="G234" s="3" t="s">
+        <v>1493</v>
+      </c>
+      <c r="H234" s="3" t="s">
+        <v>1493</v>
+      </c>
+      <c r="L234" s="3">
+        <v>40.641497907069898</v>
+      </c>
+      <c r="M234" s="3">
+        <v>14.824115014421199</v>
+      </c>
+      <c r="N234" s="3">
+        <v>2007</v>
+      </c>
+      <c r="O234" s="3">
+        <v>2</v>
+      </c>
+      <c r="P234" s="3">
+        <v>18</v>
+      </c>
+      <c r="Q234" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="V234" s="3">
+        <v>1</v>
+      </c>
+      <c r="W234" s="3" t="s">
+        <v>1494</v>
+      </c>
+      <c r="X234" s="3" t="s">
+        <v>1495</v>
+      </c>
+      <c r="Y234" s="3" t="s">
+        <v>1496</v>
+      </c>
+    </row>
+    <row r="235" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A235" s="3">
+        <v>234</v>
+      </c>
+      <c r="B235" s="3" t="s">
+        <v>1456</v>
+      </c>
+      <c r="C235" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D235" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="E235" s="3" t="s">
+        <v>1416</v>
+      </c>
+      <c r="F235" s="3" t="s">
+        <v>1417</v>
+      </c>
+      <c r="G235" s="3" t="s">
+        <v>1434</v>
+      </c>
+      <c r="H235" s="3" t="s">
+        <v>1497</v>
+      </c>
+      <c r="K235" s="10">
+        <v>50013</v>
+      </c>
+      <c r="L235" s="3">
+        <v>43.833820699411199</v>
+      </c>
+      <c r="M235" s="3">
+        <v>11.152657183193</v>
+      </c>
+      <c r="N235" s="3">
+        <v>2007</v>
+      </c>
+      <c r="O235" s="3">
+        <v>2</v>
+      </c>
+      <c r="P235" s="3">
+        <v>18</v>
+      </c>
+      <c r="Q235" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="V235" s="3">
+        <v>1</v>
+      </c>
+      <c r="W235" s="3" t="s">
+        <v>1498</v>
+      </c>
+      <c r="X235" s="3" t="s">
+        <v>1499</v>
+      </c>
+      <c r="Y235" s="3" t="s">
+        <v>1496</v>
+      </c>
+    </row>
+    <row r="236" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A236" s="3">
+        <v>235</v>
+      </c>
+      <c r="B236" s="3" t="s">
+        <v>1456</v>
+      </c>
+      <c r="C236" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D236" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="E236" s="3" t="s">
+        <v>1416</v>
+      </c>
+      <c r="F236" s="3" t="s">
+        <v>1492</v>
+      </c>
+      <c r="G236" s="3" t="s">
+        <v>1493</v>
+      </c>
+      <c r="H236" s="3" t="s">
+        <v>1500</v>
+      </c>
+      <c r="L236" s="3">
+        <v>40.755130000000001</v>
+      </c>
+      <c r="M236" s="3">
+        <v>14.7844</v>
+      </c>
+      <c r="N236" s="3">
+        <v>2007</v>
+      </c>
+      <c r="O236" s="3">
+        <v>2</v>
+      </c>
+      <c r="P236" s="3">
+        <v>18</v>
+      </c>
+      <c r="Q236" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="V236" s="3">
+        <v>1</v>
+      </c>
+      <c r="W236" s="3" t="s">
+        <v>1501</v>
+      </c>
+      <c r="X236" s="3" t="s">
+        <v>1502</v>
+      </c>
+      <c r="Y236" s="3" t="s">
+        <v>1496</v>
+      </c>
+    </row>
+    <row r="237" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A237" s="3">
+        <v>236</v>
+      </c>
+      <c r="B237" s="3" t="s">
+        <v>1456</v>
+      </c>
+      <c r="C237" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D237" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="E237" s="3" t="s">
+        <v>1416</v>
+      </c>
+      <c r="F237" s="3" t="s">
+        <v>1417</v>
+      </c>
+      <c r="G237" s="3" t="s">
+        <v>1418</v>
+      </c>
+      <c r="H237" s="3" t="s">
+        <v>1503</v>
+      </c>
+      <c r="K237" s="10" t="s">
+        <v>1504</v>
+      </c>
+      <c r="L237" s="3">
+        <v>43.5261882</v>
+      </c>
+      <c r="M237" s="3">
+        <v>10.317283099999999</v>
+      </c>
+      <c r="N237" s="3">
+        <v>2007</v>
+      </c>
+      <c r="O237" s="3">
+        <v>2</v>
+      </c>
+      <c r="P237" s="3">
+        <v>18</v>
+      </c>
+      <c r="Q237" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="V237" s="3">
+        <v>1</v>
+      </c>
+      <c r="W237" s="3" t="s">
+        <v>1505</v>
+      </c>
+      <c r="X237" s="3" t="s">
+        <v>1506</v>
+      </c>
+      <c r="Y237" s="3" t="s">
+        <v>1496</v>
+      </c>
+    </row>
+    <row r="238" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A238" s="3">
+        <v>237</v>
+      </c>
+      <c r="B238" s="3" t="s">
+        <v>1456</v>
+      </c>
+      <c r="C238" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D238" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="E238" s="3" t="s">
+        <v>1416</v>
+      </c>
+      <c r="F238" s="3" t="s">
+        <v>1465</v>
+      </c>
+      <c r="G238" s="3" t="s">
+        <v>1466</v>
+      </c>
+      <c r="H238" s="3" t="s">
+        <v>1507</v>
+      </c>
+      <c r="I238" s="3" t="s">
+        <v>1508</v>
+      </c>
+      <c r="J238" s="3" t="s">
+        <v>1509</v>
+      </c>
+      <c r="K238" s="10" t="s">
+        <v>1510</v>
+      </c>
+      <c r="L238" s="3">
+        <v>45.555827999999998</v>
+      </c>
+      <c r="M238" s="3">
+        <v>9.0619206000000005</v>
+      </c>
+      <c r="N238" s="3">
+        <v>2007</v>
+      </c>
+      <c r="O238" s="3">
+        <v>2</v>
+      </c>
+      <c r="P238" s="3">
+        <v>18</v>
+      </c>
+      <c r="Q238" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="V238" s="3">
+        <v>1</v>
+      </c>
+      <c r="W238" s="3" t="s">
+        <v>1511</v>
+      </c>
+      <c r="X238" s="3" t="s">
+        <v>1512</v>
+      </c>
+      <c r="Y238" s="3" t="s">
+        <v>1496</v>
+      </c>
+    </row>
+    <row r="239" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A239" s="3">
+        <v>238</v>
+      </c>
+      <c r="B239" s="3" t="s">
+        <v>1456</v>
+      </c>
+      <c r="C239" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D239" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="E239" s="3" t="s">
+        <v>1416</v>
+      </c>
+      <c r="F239" s="3" t="s">
+        <v>1424</v>
+      </c>
+      <c r="G239" s="3" t="s">
+        <v>1513</v>
+      </c>
+      <c r="H239" s="3" t="s">
+        <v>1514</v>
+      </c>
+      <c r="K239" s="10">
+        <v>16138</v>
+      </c>
+      <c r="L239" s="3">
+        <v>44.454373771359002</v>
+      </c>
+      <c r="M239" s="3">
+        <v>8.9751585390514101</v>
+      </c>
+      <c r="N239" s="3">
+        <v>2007</v>
+      </c>
+      <c r="O239" s="3">
+        <v>2</v>
+      </c>
+      <c r="P239" s="3">
+        <v>18</v>
+      </c>
+      <c r="Q239" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="V239" s="3">
+        <v>1</v>
+      </c>
+      <c r="W239" s="3" t="s">
+        <v>1515</v>
+      </c>
+      <c r="X239" s="3" t="s">
+        <v>1516</v>
+      </c>
+      <c r="Y239" s="3" t="s">
+        <v>1496</v>
+      </c>
+    </row>
+    <row r="240" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A240" s="3">
+        <v>239</v>
+      </c>
+      <c r="B240" s="3" t="s">
+        <v>1456</v>
+      </c>
+      <c r="C240" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D240" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="E240" s="3" t="s">
+        <v>1416</v>
+      </c>
+      <c r="F240" s="3" t="s">
+        <v>1517</v>
+      </c>
+      <c r="G240" s="3" t="s">
+        <v>1518</v>
+      </c>
+      <c r="H240" s="3" t="s">
+        <v>1519</v>
+      </c>
+      <c r="I240" s="3" t="s">
+        <v>1520</v>
+      </c>
+      <c r="J240" s="3" t="s">
+        <v>1521</v>
+      </c>
+      <c r="K240" s="10">
+        <v>42020</v>
+      </c>
+      <c r="L240" s="3">
+        <v>44.636298407341599</v>
+      </c>
+      <c r="M240" s="3">
+        <v>10.550161580296299</v>
+      </c>
+      <c r="N240" s="3">
+        <v>2007</v>
+      </c>
+      <c r="O240" s="3">
+        <v>2</v>
+      </c>
+      <c r="P240" s="3">
+        <v>18</v>
+      </c>
+      <c r="Q240" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="V240" s="3">
+        <v>1</v>
+      </c>
+      <c r="W240" s="3" t="s">
+        <v>1522</v>
+      </c>
+      <c r="X240" s="3" t="s">
+        <v>1523</v>
+      </c>
+      <c r="Y240" s="3" t="s">
+        <v>1496</v>
+      </c>
+    </row>
+    <row r="241" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A241" s="3">
+        <v>240</v>
+      </c>
+      <c r="B241" s="3" t="s">
+        <v>1456</v>
+      </c>
+      <c r="C241" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D241" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="E241" s="3" t="s">
+        <v>1416</v>
+      </c>
+      <c r="F241" s="3" t="s">
+        <v>1465</v>
+      </c>
+      <c r="G241" s="3" t="s">
+        <v>1524</v>
+      </c>
+      <c r="H241" s="3" t="s">
+        <v>1525</v>
+      </c>
+      <c r="I241" s="3" t="s">
+        <v>1526</v>
+      </c>
+      <c r="K241" s="10">
+        <v>46026</v>
+      </c>
+      <c r="L241" s="3">
+        <v>45.010540186956398</v>
+      </c>
+      <c r="M241" s="3">
+        <v>10.9886519679161</v>
+      </c>
+      <c r="N241" s="3">
+        <v>2007</v>
+      </c>
+      <c r="O241" s="3">
+        <v>2</v>
+      </c>
+      <c r="P241" s="3">
+        <v>18</v>
+      </c>
+      <c r="Q241" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="V241" s="3">
+        <v>1</v>
+      </c>
+      <c r="W241" s="3" t="s">
+        <v>1527</v>
+      </c>
+      <c r="X241" s="3" t="s">
+        <v>1528</v>
+      </c>
+      <c r="Y241" s="3" t="s">
+        <v>1496</v>
+      </c>
+    </row>
+    <row r="242" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A242" s="3">
+        <v>241</v>
+      </c>
+      <c r="B242" s="3" t="s">
+        <v>1529</v>
+      </c>
+      <c r="C242" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D242" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="E242" s="3" t="s">
+        <v>1416</v>
+      </c>
+      <c r="F242" s="3" t="s">
+        <v>1530</v>
+      </c>
+      <c r="G242" s="3" t="s">
+        <v>1531</v>
+      </c>
+      <c r="H242" s="3" t="s">
+        <v>1532</v>
+      </c>
+      <c r="K242" s="10">
+        <v>65128</v>
+      </c>
+      <c r="L242" s="3">
+        <v>42.456041503436303</v>
+      </c>
+      <c r="M242" s="3">
+        <v>14.210228000120599</v>
+      </c>
+      <c r="N242" s="3">
+        <v>2007</v>
+      </c>
+      <c r="O242" s="3">
+        <v>2</v>
+      </c>
+      <c r="P242" s="3">
+        <v>18</v>
+      </c>
+      <c r="Q242" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="V242" s="3">
+        <v>1</v>
+      </c>
+      <c r="W242" s="3" t="s">
+        <v>1533</v>
+      </c>
+      <c r="X242" s="3" t="s">
+        <v>1534</v>
+      </c>
+      <c r="Y242" s="3" t="s">
+        <v>1496</v>
+      </c>
+    </row>
+    <row r="243" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A243" s="3">
+        <v>242</v>
+      </c>
+      <c r="B243" s="3" t="s">
+        <v>1529</v>
+      </c>
+      <c r="C243" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D243" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="E243" s="3" t="s">
+        <v>1416</v>
+      </c>
+      <c r="F243" s="3" t="s">
+        <v>1517</v>
+      </c>
+      <c r="G243" s="3" t="s">
+        <v>1535</v>
+      </c>
+      <c r="H243" s="3" t="s">
+        <v>1536</v>
+      </c>
+      <c r="I243" s="3" t="s">
+        <v>1537</v>
+      </c>
+      <c r="K243" s="10">
+        <v>47021</v>
+      </c>
+      <c r="L243" s="3">
+        <v>43.858572330741801</v>
+      </c>
+      <c r="M243" s="3">
+        <v>11.975318391182499</v>
+      </c>
+      <c r="N243" s="3">
+        <v>2007</v>
+      </c>
+      <c r="O243" s="3">
+        <v>2</v>
+      </c>
+      <c r="P243" s="3">
+        <v>18</v>
+      </c>
+      <c r="Q243" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="V243" s="3">
+        <v>1</v>
+      </c>
+      <c r="W243" s="3" t="s">
+        <v>1538</v>
+      </c>
+      <c r="X243" s="3" t="s">
+        <v>1539</v>
+      </c>
+      <c r="Y243" s="3" t="s">
+        <v>1496</v>
+      </c>
+    </row>
+    <row r="244" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A244" s="3">
+        <v>243</v>
+      </c>
+      <c r="B244" s="3" t="s">
+        <v>1529</v>
+      </c>
+      <c r="C244" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D244" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="E244" s="3" t="s">
+        <v>1416</v>
+      </c>
+      <c r="F244" s="3" t="s">
+        <v>1424</v>
+      </c>
+      <c r="G244" s="3" t="s">
+        <v>1513</v>
+      </c>
+      <c r="H244" s="3" t="s">
+        <v>1540</v>
+      </c>
+      <c r="I244" s="3" t="s">
+        <v>1541</v>
+      </c>
+      <c r="J244" s="3" t="s">
+        <v>1542</v>
+      </c>
+      <c r="K244" s="10">
+        <v>16011</v>
+      </c>
+      <c r="L244" s="3">
+        <v>44.403024364921002</v>
+      </c>
+      <c r="M244" s="3">
+        <v>8.6844438959323007</v>
+      </c>
+      <c r="N244" s="3">
+        <v>2007</v>
+      </c>
+      <c r="O244" s="3">
+        <v>2</v>
+      </c>
+      <c r="P244" s="3">
+        <v>18</v>
+      </c>
+      <c r="Q244" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="V244" s="3">
+        <v>1</v>
+      </c>
+      <c r="W244" s="3" t="s">
+        <v>1543</v>
+      </c>
+      <c r="X244" s="3" t="s">
+        <v>1544</v>
+      </c>
+      <c r="Y244" s="3" t="s">
+        <v>1496</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Germany data and source code improvements
</commit_message>
<xml_diff>
--- a/a-place-for-salvador-allende/a_place_for_salvador_allende.xlsx
+++ b/a-place-for-salvador-allende/a_place_for_salvador_allende.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://onemsci-my.sharepoint.com/personal/glo_canonoy_msci_com/Documents/03 Training/datasets-of-interest/a-place-for-salvador-allende/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1720" documentId="11_FF6F299C653B866D72320E251CEDB2C4009A2F63" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{466FB066-35A2-4762-8820-79721BFEB978}"/>
+  <xr:revisionPtr revIDLastSave="1742" documentId="11_FF6F299C653B866D72320E251CEDB2C4009A2F63" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02044F7E-408F-45C5-A970-141E68910E42}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="allende" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">allende!$B$1:$AO$286</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">allende!$B$1:$AO$309</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3525" uniqueCount="1762">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3819" uniqueCount="1913">
   <si>
     <t>id</t>
   </si>
@@ -5570,6 +5570,502 @@
 In memoria di Salvador Allende  e di tutte le vittime della dittatura cilena "1973 - 1989" di Pinochet
 Lastra a Signa 27.1.2004 - 
 Comune Di Lastra A Signa - Comitato Dei Lavoratori Cileni Esiliati</t>
+  </si>
+  <si>
+    <t>Salvador-Allende-Straße</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Treptow-Köpenick</t>
+  </si>
+  <si>
+    <t>Köpenick</t>
+  </si>
+  <si>
+    <t>Salvador-Allende-Viertel I</t>
+  </si>
+  <si>
+    <t>12559</t>
+  </si>
+  <si>
+    <t>Dr. Salvador Allende Gossens
+Präsident der Republik Chile
+Träger des internationalen Lenin-[...]
+geboren am 26. Juni 1908
+ermordet am 11. September 1973</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/1155000864</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/LbxT436ydEK3N65eA</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2009/11/08/436-berlin-alemania</t>
+  </si>
+  <si>
+    <t>Denkmal Salvador Allende</t>
+  </si>
+  <si>
+    <t>Pablo-Neruda-Straße</t>
+  </si>
+  <si>
+    <t>Salvador Allende
+*26.06.1908 in Valparaiso (Chile), 
+†11.09.1973 in Santiago de Chile
+Arzt
+Mitglied der Sozialistischen Partei von Chile 
+1970 zum Präsidenten der Republik Chile gewählt
+1973 durch einen Putsch des Militärs unter General Pinochet gestürzt. Nach Erstürmung des Präsidenten-palastes Moneda durch das Militär beging er Selbstmord.
+Vor der Moneda steht heute ein Denkmal für ihn.
+Werktätige meines Vaterlandes! Ich möchte euch danken für die Loyalität, die ihr immer bewiesen habt, für das Vertrauen, das ihr in einen Mann gesetzt habt, der nur der Dolmetscher der großen Bestrebungen nach Gerechtigkeit war, der sich in seinen Erklärungen verpflichtet hat, die Verfassung und das Gesetz zu respektieren, und der seiner Verpflichtung treu war.
+Radio Magallanes wird sicherlich zum Schweigen gebracht werden, und der ruhige Ton meiner Stimme wird euch nicht mehr erreichen. Das macht nichts, ihr werdet sie weiter hören, ich werde immer mit euch sein, und ich werde zumindest die Erinnerung an einen würdigen Menschen hinterlassen, der loyal war hinsichtlich der Loyalität zu den Werktätigen.
+(Aus der Rede von Salvador Allende über Radio Magallanes am 11.09.1973, währenddessen der Präsidentenpalast bombardiert wurde)
+Pablo Neruda
+*12.07.1904 in Parral (Chile),
+†23.09.1973 in Santiago de Chile
+Dichter
+Mitglied der Kommunistischen Partei von Chile
+Viele Jahre Senator der Republik Chile
+Während der Präsidentschaft Salvador Allendes Botschafter der Republik Chile in Paris
+Nobelpreisträger für Literatur (1971)
+Wo immer ich war, auch in den fernsten Ländern, 
+bewunderten die Völker den Präsidenten Allende und rühmten den 
+außerordentlichen Pluralismus unserer Regierung.
+Hier, in Chile, wurde unter ungeheuren Schwierigkeiten eine 
+wahrhaft gerechte Gesellschaft aufgebaut, 
+errichtet auf der Grundlage unserer Souveränität,
+unseres Nationalstolzes,
+des Heldentums der besten Einwohner Chiles.
+Auf unserer Seite, auf der Seite der chilenischen Revolution, 
+waren die Verfassung und das Gesetz,
+die Demokratie und die Hoffnung.
+(Pablo Neruda: Ich bekenne ich habe gelebt. Memoiren 1973)
+Zeichnungen
+Walter Woche (Zyklus „In Chile herrscht Ruhe‟, Berlin, 1973/1974)
+mit freundlicher Genehmigung von Hanny Womacka
+Die Büste von Salvador Allende schuf Dietrich Rohde (Berlin, 1981), sie wurde 1983 auf dem Hof der damaligen Salvador-Allende-Oberschule (heute Emmy-Noether-Gymnasium) enthüllt, nach 1990 vor den Eingang der Schule und jetzt ins Allende-Viertel gerückt.
+Eigentum des Bezirksamtes Treptow-Köpenick von Berlin</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/node/6467775271</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/35WNNez4fJHL6fpo8</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2012/07/19/575-berlin-alemania</t>
+  </si>
+  <si>
+    <t>Free Hanseatic City of Bremen</t>
+  </si>
+  <si>
+    <t>Bremen</t>
+  </si>
+  <si>
+    <t>Bremen-Mitte</t>
+  </si>
+  <si>
+    <t>Mitte</t>
+  </si>
+  <si>
+    <t>Ostertor</t>
+  </si>
+  <si>
+    <t>28203</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/316139440</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/YykDLWhopkCkUt1x5</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2012/06/25/571-bremen-alemania</t>
+  </si>
+  <si>
+    <t>Saxony</t>
+  </si>
+  <si>
+    <t>Dresden</t>
+  </si>
+  <si>
+    <t>Plauen</t>
+  </si>
+  <si>
+    <t>Südvorstadt</t>
+  </si>
+  <si>
+    <t>Südvorstadt-West</t>
+  </si>
+  <si>
+    <t>01187</t>
+  </si>
+  <si>
+    <t>Salvador Allende
+Vom Volk gewählter Präsident Chiles / Ermordet von einer reaktionären Militärjunta am 11. September 1973</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/node/300860595</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2009/01/14/302-dresde-alemania</t>
+  </si>
+  <si>
+    <t>Allende-Platz</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Eimsbüttel</t>
+  </si>
+  <si>
+    <t>Rotherbaum</t>
+  </si>
+  <si>
+    <t>20146</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allende-Platz
+Dr. Salvador A. (1908-1973)
+Demokratisch gewählter, von Putschisten ermordeter Präsident Chiles. 
+</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/relation/206474</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/VSxbAKjcAJNq1iHb7</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2007/02/18/35-hamburgo-alemania</t>
+  </si>
+  <si>
+    <t>Dr.-Salvador-Allende-Straße</t>
+  </si>
+  <si>
+    <t>Bautzen</t>
+  </si>
+  <si>
+    <t>Bautzen - Budyšin</t>
+  </si>
+  <si>
+    <t>Ostvorstadt - Wuchodne předměsto</t>
+  </si>
+  <si>
+    <t>Wichmannsiedlung</t>
+  </si>
+  <si>
+    <t>02625</t>
+  </si>
+  <si>
+    <t>Dr. Salvador Allende Präsident des Chilenischen Volkes ermordet am 11.9.1973 von Faschistischer Militärjunta</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/25884604</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/iTWTgyLUsY2VbQLP9</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2008/12/13/295-bautzen-alemania</t>
+  </si>
+  <si>
+    <t>Bavaria</t>
+  </si>
+  <si>
+    <t>Nuremberg</t>
+  </si>
+  <si>
+    <t>Eibach</t>
+  </si>
+  <si>
+    <t>90451</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/27224506</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/FAgWf1YzQMzXdKbP8</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2009/10/12/424-nuremburgo-alemania</t>
+  </si>
+  <si>
+    <t>Mecklenburg-Vorpommern</t>
+  </si>
+  <si>
+    <t>Mecklenburgische Seenplatte</t>
+  </si>
+  <si>
+    <t>Neubrandenburg</t>
+  </si>
+  <si>
+    <t>Oststadt</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/315259423</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/NyTkrGRn12nsWqF6A</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2007/02/18/23-alemania</t>
+  </si>
+  <si>
+    <t>Thuringia</t>
+  </si>
+  <si>
+    <t>Weimar</t>
+  </si>
+  <si>
+    <t>Westvorstadt</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/142282000</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/ALKvidsgLW3toJzx5</t>
+  </si>
+  <si>
+    <t>Erfurt</t>
+  </si>
+  <si>
+    <t>Rostock</t>
+  </si>
+  <si>
+    <t>Ortsbeirat 18 : Toitenwinkel</t>
+  </si>
+  <si>
+    <t>Toitenwinkel</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/4790712</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/n98BzehjpY8CX1SY9</t>
+  </si>
+  <si>
+    <t>Brandenburg</t>
+  </si>
+  <si>
+    <t>Teltow-Fläming</t>
+  </si>
+  <si>
+    <t>Ludwigsfelde</t>
+  </si>
+  <si>
+    <t>Industriepark-West</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/254878894</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/bsPMnnTeSeCgnu3q9</t>
+  </si>
+  <si>
+    <t>Dr.-Salvador-Allende-Siedlung</t>
+  </si>
+  <si>
+    <t>Vorpommern-Greifswald</t>
+  </si>
+  <si>
+    <t>Torgelow-Ferdinandshof</t>
+  </si>
+  <si>
+    <t>Torgelow</t>
+  </si>
+  <si>
+    <t>Spechtberg</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/57996675</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/dbVqHaoMQstjwYNs9</t>
+  </si>
+  <si>
+    <t>Chemnitz</t>
+  </si>
+  <si>
+    <t>Kappel</t>
+  </si>
+  <si>
+    <t>Wohngebiet Fritz Heckert</t>
+  </si>
+  <si>
+    <t>09119</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/4598959</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/2UrvCwzUmNUdyQCZA</t>
+  </si>
+  <si>
+    <t>Dr.-Salvador-Allende-Grundschule</t>
+  </si>
+  <si>
+    <t>Straße Usti nad Labem</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/92663471</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/RDn2QsQTvwELDDxPA</t>
+  </si>
+  <si>
+    <t>Saxony-Anhalt</t>
+  </si>
+  <si>
+    <t>Magdeburg</t>
+  </si>
+  <si>
+    <t>Neustädter See</t>
+  </si>
+  <si>
+    <t>39126</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/8589834</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/tEjrJ9vPtC3SpJVH8</t>
+  </si>
+  <si>
+    <t>Salvador-Allende-Platz / Stadtteilzentrum Dr. Salvador Allende</t>
+  </si>
+  <si>
+    <t>Jena</t>
+  </si>
+  <si>
+    <t>Neulobeda</t>
+  </si>
+  <si>
+    <t>Lobeda Ost</t>
+  </si>
+  <si>
+    <t>07747</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/221260808</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/7SkDDAVu7KvWfa6b7</t>
+  </si>
+  <si>
+    <t>Emmy-Noether-Gymnasium</t>
+  </si>
+  <si>
+    <t>Salvador-Allende-Oberschule</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/214614429</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/oYGeSnqbKecCBkG36</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2008/12/01/289-berlin-alemania</t>
+  </si>
+  <si>
+    <t>Salvador-Allende-Viertel</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/148738458</t>
+  </si>
+  <si>
+    <t>Salvador-Allende-Haus</t>
+  </si>
+  <si>
+    <t>North Rhine-Westphalia</t>
+  </si>
+  <si>
+    <t>Kreis Recklinghausen</t>
+  </si>
+  <si>
+    <t>Oer-Erkenschwick</t>
+  </si>
+  <si>
+    <t>Oer</t>
+  </si>
+  <si>
+    <t>Haardgrenzweg</t>
+  </si>
+  <si>
+    <t>45739</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/node/1026703443</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2009/07/27/384-oer-erkenschwick-alemania</t>
+  </si>
+  <si>
+    <t>Dr-Salvador-Allende-Schule</t>
+  </si>
+  <si>
+    <t>Ostprignitz-Ruppin</t>
+  </si>
+  <si>
+    <t>Rheinsberg</t>
+  </si>
+  <si>
+    <t>Kiefernweg</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/ZMrPyxSWMdhJUtvw9</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2009/06/16/360-rheinsberg-alemania</t>
+  </si>
+  <si>
+    <t>Ruins of FDGB-Erholungsheim Salvador Allende</t>
+  </si>
+  <si>
+    <t>others</t>
+  </si>
+  <si>
+    <t>Uckermark</t>
+  </si>
+  <si>
+    <t>Templin</t>
+  </si>
+  <si>
+    <t>FDGB-Erholungsheim Salvador Allende</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2008/05/11/189-templin-alemania</t>
+  </si>
+  <si>
+    <t>Ganztags-Sekundarschule "Dr. Salvador Allende"</t>
+  </si>
+  <si>
+    <t>Altmarkkreis Salzwedel</t>
+  </si>
+  <si>
+    <t>Klötze</t>
+  </si>
+  <si>
+    <t>Straße der Jugend</t>
+  </si>
+  <si>
+    <t>38486</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/32961537</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/gWYEWYvB8sEZk7bV9</t>
+  </si>
+  <si>
+    <t>http://www.abacq.org/calle/index.php?2007/10/22/123-klotze-alemania</t>
   </si>
 </sst>
 </file>
@@ -5904,13 +6400,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AO286"/>
+  <dimension ref="A1:AO309"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B272" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B296" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A287" sqref="A287"/>
+      <selection pane="bottomRight" activeCell="A310" sqref="A310"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -15371,16 +15867,10 @@
         <v>4.8122349896955399</v>
       </c>
       <c r="N151" s="3">
-        <v>2007</v>
-      </c>
-      <c r="O151" s="3">
-        <v>2</v>
-      </c>
-      <c r="P151" s="3">
-        <v>18</v>
+        <v>1974</v>
       </c>
       <c r="Q151" s="3" t="s">
-        <v>441</v>
+        <v>965</v>
       </c>
       <c r="R151" s="3" t="s">
         <v>901</v>
@@ -18679,6 +19169,7 @@
       <c r="Q205" s="3" t="s">
         <v>443</v>
       </c>
+      <c r="R205" s="16"/>
       <c r="V205" s="3">
         <v>1</v>
       </c>
@@ -23645,8 +24136,1389 @@
         <v>1691</v>
       </c>
     </row>
+    <row r="287" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A287" s="3">
+        <v>286</v>
+      </c>
+      <c r="B287" s="3" t="s">
+        <v>1762</v>
+      </c>
+      <c r="C287" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D287" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="E287" s="3" t="s">
+        <v>1763</v>
+      </c>
+      <c r="F287" s="3" t="s">
+        <v>1764</v>
+      </c>
+      <c r="G287" s="3" t="s">
+        <v>1765</v>
+      </c>
+      <c r="H287" s="3" t="s">
+        <v>1766</v>
+      </c>
+      <c r="I287" s="3" t="s">
+        <v>1767</v>
+      </c>
+      <c r="K287" s="10" t="s">
+        <v>1768</v>
+      </c>
+      <c r="L287" s="3">
+        <v>52.442599999999999</v>
+      </c>
+      <c r="M287" s="3">
+        <v>13.59018</v>
+      </c>
+      <c r="N287" s="3">
+        <v>1973</v>
+      </c>
+      <c r="O287" s="3">
+        <v>11</v>
+      </c>
+      <c r="P287" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q287" s="3" t="s">
+        <v>965</v>
+      </c>
+      <c r="R287" s="3" t="s">
+        <v>1769</v>
+      </c>
+      <c r="S287" s="3" t="s">
+        <v>666</v>
+      </c>
+      <c r="V287" s="3">
+        <v>1</v>
+      </c>
+      <c r="W287" s="3" t="s">
+        <v>1770</v>
+      </c>
+      <c r="X287" s="3" t="s">
+        <v>1771</v>
+      </c>
+      <c r="Y287" s="3" t="s">
+        <v>1772</v>
+      </c>
+    </row>
+    <row r="288" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A288" s="3">
+        <v>287</v>
+      </c>
+      <c r="B288" s="3" t="s">
+        <v>1773</v>
+      </c>
+      <c r="C288" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D288" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="E288" s="3" t="s">
+        <v>1763</v>
+      </c>
+      <c r="F288" s="3" t="s">
+        <v>1764</v>
+      </c>
+      <c r="G288" s="3" t="s">
+        <v>1765</v>
+      </c>
+      <c r="H288" s="3" t="s">
+        <v>1766</v>
+      </c>
+      <c r="I288" s="3" t="s">
+        <v>1767</v>
+      </c>
+      <c r="J288" s="3" t="s">
+        <v>1774</v>
+      </c>
+      <c r="K288" s="10" t="s">
+        <v>1768</v>
+      </c>
+      <c r="L288" s="3">
+        <v>52.442656599999999</v>
+      </c>
+      <c r="M288" s="3">
+        <v>13.589798099999999</v>
+      </c>
+      <c r="N288" s="3">
+        <v>1981</v>
+      </c>
+      <c r="Q288" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="R288" s="3" t="s">
+        <v>1775</v>
+      </c>
+      <c r="S288" s="3" t="s">
+        <v>666</v>
+      </c>
+      <c r="V288" s="3">
+        <v>1</v>
+      </c>
+      <c r="W288" s="3" t="s">
+        <v>1776</v>
+      </c>
+      <c r="X288" s="3" t="s">
+        <v>1777</v>
+      </c>
+      <c r="Y288" s="3" t="s">
+        <v>1778</v>
+      </c>
+    </row>
+    <row r="289" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A289" s="3">
+        <v>288</v>
+      </c>
+      <c r="B289" s="3" t="s">
+        <v>1762</v>
+      </c>
+      <c r="C289" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D289" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="E289" s="3" t="s">
+        <v>1763</v>
+      </c>
+      <c r="F289" s="3" t="s">
+        <v>1779</v>
+      </c>
+      <c r="G289" s="3" t="s">
+        <v>1780</v>
+      </c>
+      <c r="H289" s="3" t="s">
+        <v>1781</v>
+      </c>
+      <c r="I289" s="3" t="s">
+        <v>1782</v>
+      </c>
+      <c r="J289" s="3" t="s">
+        <v>1783</v>
+      </c>
+      <c r="K289" s="10" t="s">
+        <v>1784</v>
+      </c>
+      <c r="L289" s="3">
+        <v>53.0756005</v>
+      </c>
+      <c r="M289" s="3">
+        <v>8.8177029000000005</v>
+      </c>
+      <c r="N289" s="3">
+        <v>2007</v>
+      </c>
+      <c r="O289" s="3">
+        <v>2</v>
+      </c>
+      <c r="P289" s="3">
+        <v>18</v>
+      </c>
+      <c r="Q289" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="V289" s="3">
+        <v>1</v>
+      </c>
+      <c r="W289" s="3" t="s">
+        <v>1785</v>
+      </c>
+      <c r="X289" s="3" t="s">
+        <v>1786</v>
+      </c>
+      <c r="Y289" s="3" t="s">
+        <v>1787</v>
+      </c>
+    </row>
+    <row r="290" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A290" s="3">
+        <v>289</v>
+      </c>
+      <c r="B290" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C290" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D290" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="E290" s="3" t="s">
+        <v>1763</v>
+      </c>
+      <c r="F290" s="3" t="s">
+        <v>1788</v>
+      </c>
+      <c r="G290" s="3" t="s">
+        <v>1789</v>
+      </c>
+      <c r="H290" s="3" t="s">
+        <v>1790</v>
+      </c>
+      <c r="I290" s="3" t="s">
+        <v>1791</v>
+      </c>
+      <c r="J290" s="3" t="s">
+        <v>1792</v>
+      </c>
+      <c r="K290" s="10" t="s">
+        <v>1793</v>
+      </c>
+      <c r="L290" s="3">
+        <v>51.0297032</v>
+      </c>
+      <c r="M290" s="3">
+        <v>13.7217862</v>
+      </c>
+      <c r="N290" s="3">
+        <v>1973</v>
+      </c>
+      <c r="O290" s="3">
+        <v>11</v>
+      </c>
+      <c r="P290" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q290" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="R290" s="3" t="s">
+        <v>1794</v>
+      </c>
+      <c r="S290" s="3" t="s">
+        <v>666</v>
+      </c>
+      <c r="V290" s="3">
+        <v>1</v>
+      </c>
+      <c r="W290" s="3" t="s">
+        <v>1795</v>
+      </c>
+      <c r="Y290" s="3" t="s">
+        <v>1796</v>
+      </c>
+    </row>
+    <row r="291" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A291" s="3">
+        <v>290</v>
+      </c>
+      <c r="B291" s="3" t="s">
+        <v>1797</v>
+      </c>
+      <c r="C291" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D291" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="E291" s="3" t="s">
+        <v>1763</v>
+      </c>
+      <c r="F291" s="3" t="s">
+        <v>1798</v>
+      </c>
+      <c r="G291" s="3" t="s">
+        <v>1799</v>
+      </c>
+      <c r="H291" s="3" t="s">
+        <v>1800</v>
+      </c>
+      <c r="K291" s="10" t="s">
+        <v>1801</v>
+      </c>
+      <c r="L291" s="3">
+        <v>53.567681999999998</v>
+      </c>
+      <c r="M291" s="3">
+        <v>9.9830111956519296</v>
+      </c>
+      <c r="N291" s="3">
+        <v>2007</v>
+      </c>
+      <c r="O291" s="3">
+        <v>2</v>
+      </c>
+      <c r="P291" s="3">
+        <v>18</v>
+      </c>
+      <c r="Q291" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="R291" s="3" t="s">
+        <v>1802</v>
+      </c>
+      <c r="S291" s="3" t="s">
+        <v>666</v>
+      </c>
+      <c r="V291" s="3">
+        <v>1</v>
+      </c>
+      <c r="W291" s="3" t="s">
+        <v>1803</v>
+      </c>
+      <c r="X291" s="3" t="s">
+        <v>1804</v>
+      </c>
+      <c r="Y291" s="3" t="s">
+        <v>1805</v>
+      </c>
+    </row>
+    <row r="292" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A292" s="3">
+        <v>291</v>
+      </c>
+      <c r="B292" s="3" t="s">
+        <v>1806</v>
+      </c>
+      <c r="C292" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D292" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="E292" s="3" t="s">
+        <v>1763</v>
+      </c>
+      <c r="F292" s="3" t="s">
+        <v>1788</v>
+      </c>
+      <c r="G292" s="3" t="s">
+        <v>1807</v>
+      </c>
+      <c r="H292" s="3" t="s">
+        <v>1808</v>
+      </c>
+      <c r="I292" s="3" t="s">
+        <v>1809</v>
+      </c>
+      <c r="J292" s="3" t="s">
+        <v>1810</v>
+      </c>
+      <c r="K292" s="10" t="s">
+        <v>1811</v>
+      </c>
+      <c r="L292" s="3">
+        <v>51.174043599999997</v>
+      </c>
+      <c r="M292" s="3">
+        <v>14.4580679</v>
+      </c>
+      <c r="N292" s="3">
+        <v>1973</v>
+      </c>
+      <c r="O292" s="3">
+        <v>11</v>
+      </c>
+      <c r="Q292" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="R292" s="3" t="s">
+        <v>1812</v>
+      </c>
+      <c r="S292" s="3" t="s">
+        <v>666</v>
+      </c>
+      <c r="V292" s="3">
+        <v>1</v>
+      </c>
+      <c r="W292" s="3" t="s">
+        <v>1813</v>
+      </c>
+      <c r="X292" s="3" t="s">
+        <v>1814</v>
+      </c>
+      <c r="Y292" s="3" t="s">
+        <v>1815</v>
+      </c>
+    </row>
+    <row r="293" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A293" s="3">
+        <v>292</v>
+      </c>
+      <c r="B293" s="3" t="s">
+        <v>1762</v>
+      </c>
+      <c r="C293" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D293" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="E293" s="3" t="s">
+        <v>1763</v>
+      </c>
+      <c r="F293" s="3" t="s">
+        <v>1816</v>
+      </c>
+      <c r="G293" s="3" t="s">
+        <v>1817</v>
+      </c>
+      <c r="H293" s="3" t="s">
+        <v>1818</v>
+      </c>
+      <c r="K293" s="10" t="s">
+        <v>1819</v>
+      </c>
+      <c r="L293" s="3">
+        <v>49.413352099999997</v>
+      </c>
+      <c r="M293" s="3">
+        <v>11.038062399999999</v>
+      </c>
+      <c r="N293" s="3">
+        <v>2008</v>
+      </c>
+      <c r="O293" s="3">
+        <v>8</v>
+      </c>
+      <c r="Q293" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="V293" s="3">
+        <v>1</v>
+      </c>
+      <c r="W293" s="3" t="s">
+        <v>1820</v>
+      </c>
+      <c r="X293" s="3" t="s">
+        <v>1821</v>
+      </c>
+      <c r="Y293" s="3" t="s">
+        <v>1822</v>
+      </c>
+    </row>
+    <row r="294" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A294" s="3">
+        <v>293</v>
+      </c>
+      <c r="B294" s="3" t="s">
+        <v>1762</v>
+      </c>
+      <c r="C294" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D294" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="E294" s="3" t="s">
+        <v>1763</v>
+      </c>
+      <c r="F294" s="3" t="s">
+        <v>1823</v>
+      </c>
+      <c r="G294" s="3" t="s">
+        <v>1824</v>
+      </c>
+      <c r="H294" s="3" t="s">
+        <v>1825</v>
+      </c>
+      <c r="I294" s="3" t="s">
+        <v>1826</v>
+      </c>
+      <c r="K294" s="10">
+        <v>17036</v>
+      </c>
+      <c r="L294" s="3">
+        <v>53.550460000000001</v>
+      </c>
+      <c r="M294" s="3">
+        <v>13.292289999999999</v>
+      </c>
+      <c r="N294" s="3">
+        <v>2007</v>
+      </c>
+      <c r="O294" s="3">
+        <v>2</v>
+      </c>
+      <c r="P294" s="3">
+        <v>18</v>
+      </c>
+      <c r="Q294" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="V294" s="3">
+        <v>1</v>
+      </c>
+      <c r="W294" s="3" t="s">
+        <v>1827</v>
+      </c>
+      <c r="X294" s="3" t="s">
+        <v>1828</v>
+      </c>
+      <c r="Y294" s="3" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="295" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A295" s="3">
+        <v>294</v>
+      </c>
+      <c r="B295" s="3" t="s">
+        <v>1806</v>
+      </c>
+      <c r="C295" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D295" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="E295" s="3" t="s">
+        <v>1763</v>
+      </c>
+      <c r="F295" s="3" t="s">
+        <v>1830</v>
+      </c>
+      <c r="G295" s="3" t="s">
+        <v>1831</v>
+      </c>
+      <c r="H295" s="3" t="s">
+        <v>1832</v>
+      </c>
+      <c r="K295" s="10">
+        <v>99425</v>
+      </c>
+      <c r="L295" s="3">
+        <v>50.974899999999998</v>
+      </c>
+      <c r="M295" s="3">
+        <v>11.31185</v>
+      </c>
+      <c r="N295" s="3">
+        <v>2007</v>
+      </c>
+      <c r="O295" s="3">
+        <v>2</v>
+      </c>
+      <c r="P295" s="3">
+        <v>18</v>
+      </c>
+      <c r="Q295" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="V295" s="3">
+        <v>1</v>
+      </c>
+      <c r="W295" s="3" t="s">
+        <v>1833</v>
+      </c>
+      <c r="X295" s="3" t="s">
+        <v>1834</v>
+      </c>
+      <c r="Y295" s="3" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="296" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A296" s="3">
+        <v>295</v>
+      </c>
+      <c r="B296" s="3" t="s">
+        <v>1762</v>
+      </c>
+      <c r="C296" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D296" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="E296" s="3" t="s">
+        <v>1763</v>
+      </c>
+      <c r="F296" s="3" t="s">
+        <v>1835</v>
+      </c>
+      <c r="N296" s="3">
+        <v>2007</v>
+      </c>
+      <c r="O296" s="3">
+        <v>2</v>
+      </c>
+      <c r="P296" s="3">
+        <v>18</v>
+      </c>
+      <c r="Q296" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="V296" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y296" s="3" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="297" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A297" s="3">
+        <v>296</v>
+      </c>
+      <c r="B297" s="3" t="s">
+        <v>1762</v>
+      </c>
+      <c r="C297" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D297" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="E297" s="3" t="s">
+        <v>1763</v>
+      </c>
+      <c r="F297" s="3" t="s">
+        <v>1823</v>
+      </c>
+      <c r="G297" s="3" t="s">
+        <v>1836</v>
+      </c>
+      <c r="H297" s="3" t="s">
+        <v>1837</v>
+      </c>
+      <c r="I297" s="3" t="s">
+        <v>1838</v>
+      </c>
+      <c r="K297" s="10">
+        <v>18147</v>
+      </c>
+      <c r="L297" s="3">
+        <v>54.117319999999999</v>
+      </c>
+      <c r="M297" s="3">
+        <v>12.147</v>
+      </c>
+      <c r="N297" s="3">
+        <v>2007</v>
+      </c>
+      <c r="O297" s="3">
+        <v>2</v>
+      </c>
+      <c r="P297" s="3">
+        <v>18</v>
+      </c>
+      <c r="Q297" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="V297" s="3">
+        <v>1</v>
+      </c>
+      <c r="W297" s="3" t="s">
+        <v>1839</v>
+      </c>
+      <c r="X297" s="3" t="s">
+        <v>1840</v>
+      </c>
+      <c r="Y297" s="3" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="298" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A298" s="3">
+        <v>297</v>
+      </c>
+      <c r="B298" s="3" t="s">
+        <v>1762</v>
+      </c>
+      <c r="C298" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D298" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="E298" s="3" t="s">
+        <v>1763</v>
+      </c>
+      <c r="F298" s="3" t="s">
+        <v>1841</v>
+      </c>
+      <c r="G298" s="3" t="s">
+        <v>1842</v>
+      </c>
+      <c r="H298" s="3" t="s">
+        <v>1843</v>
+      </c>
+      <c r="I298" s="3" t="s">
+        <v>1844</v>
+      </c>
+      <c r="K298" s="10">
+        <v>14974</v>
+      </c>
+      <c r="L298" s="3">
+        <v>52.306620000000002</v>
+      </c>
+      <c r="M298" s="3">
+        <v>13.246359999999999</v>
+      </c>
+      <c r="N298" s="3">
+        <v>2007</v>
+      </c>
+      <c r="O298" s="3">
+        <v>2</v>
+      </c>
+      <c r="P298" s="3">
+        <v>18</v>
+      </c>
+      <c r="Q298" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="V298" s="3">
+        <v>1</v>
+      </c>
+      <c r="W298" s="3" t="s">
+        <v>1845</v>
+      </c>
+      <c r="X298" s="3" t="s">
+        <v>1846</v>
+      </c>
+      <c r="Y298" s="3" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="299" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A299" s="3">
+        <v>298</v>
+      </c>
+      <c r="B299" s="3" t="s">
+        <v>1847</v>
+      </c>
+      <c r="C299" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D299" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="E299" s="3" t="s">
+        <v>1763</v>
+      </c>
+      <c r="F299" s="3" t="s">
+        <v>1823</v>
+      </c>
+      <c r="G299" s="3" t="s">
+        <v>1848</v>
+      </c>
+      <c r="H299" s="3" t="s">
+        <v>1849</v>
+      </c>
+      <c r="I299" s="3" t="s">
+        <v>1850</v>
+      </c>
+      <c r="J299" s="3" t="s">
+        <v>1851</v>
+      </c>
+      <c r="K299" s="10">
+        <v>17358</v>
+      </c>
+      <c r="L299" s="3">
+        <v>53.636780000000002</v>
+      </c>
+      <c r="M299" s="3">
+        <v>14.011570000000001</v>
+      </c>
+      <c r="N299" s="3">
+        <v>2007</v>
+      </c>
+      <c r="O299" s="3">
+        <v>2</v>
+      </c>
+      <c r="P299" s="3">
+        <v>18</v>
+      </c>
+      <c r="Q299" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="V299" s="3">
+        <v>1</v>
+      </c>
+      <c r="W299" s="3" t="s">
+        <v>1852</v>
+      </c>
+      <c r="X299" s="3" t="s">
+        <v>1853</v>
+      </c>
+      <c r="Y299" s="3" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="300" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A300" s="3">
+        <v>299</v>
+      </c>
+      <c r="B300" s="3" t="s">
+        <v>1806</v>
+      </c>
+      <c r="C300" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D300" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="E300" s="3" t="s">
+        <v>1763</v>
+      </c>
+      <c r="F300" s="3" t="s">
+        <v>1788</v>
+      </c>
+      <c r="G300" s="3" t="s">
+        <v>1854</v>
+      </c>
+      <c r="H300" s="3" t="s">
+        <v>1855</v>
+      </c>
+      <c r="I300" s="3" t="s">
+        <v>1856</v>
+      </c>
+      <c r="K300" s="10" t="s">
+        <v>1857</v>
+      </c>
+      <c r="L300" s="3">
+        <v>50.804229999999997</v>
+      </c>
+      <c r="M300" s="3">
+        <v>12.886979999999999</v>
+      </c>
+      <c r="N300" s="3">
+        <v>2007</v>
+      </c>
+      <c r="O300" s="3">
+        <v>2</v>
+      </c>
+      <c r="P300" s="3">
+        <v>18</v>
+      </c>
+      <c r="Q300" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="V300" s="3">
+        <v>1</v>
+      </c>
+      <c r="W300" s="3" t="s">
+        <v>1858</v>
+      </c>
+      <c r="X300" s="3" t="s">
+        <v>1859</v>
+      </c>
+      <c r="Y300" s="3" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="301" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A301" s="3">
+        <v>300</v>
+      </c>
+      <c r="B301" s="3" t="s">
+        <v>1860</v>
+      </c>
+      <c r="C301" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D301" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="E301" s="3" t="s">
+        <v>1763</v>
+      </c>
+      <c r="F301" s="3" t="s">
+        <v>1788</v>
+      </c>
+      <c r="G301" s="3" t="s">
+        <v>1854</v>
+      </c>
+      <c r="H301" s="3" t="s">
+        <v>1855</v>
+      </c>
+      <c r="I301" s="3" t="s">
+        <v>1856</v>
+      </c>
+      <c r="J301" s="3" t="s">
+        <v>1861</v>
+      </c>
+      <c r="K301" s="10" t="s">
+        <v>1857</v>
+      </c>
+      <c r="L301" s="3">
+        <v>50.8052701981822</v>
+      </c>
+      <c r="M301" s="3">
+        <v>12.8851103621978</v>
+      </c>
+      <c r="N301" s="3">
+        <v>2007</v>
+      </c>
+      <c r="O301" s="3">
+        <v>2</v>
+      </c>
+      <c r="P301" s="3">
+        <v>18</v>
+      </c>
+      <c r="Q301" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="V301" s="3">
+        <v>1</v>
+      </c>
+      <c r="W301" s="3" t="s">
+        <v>1862</v>
+      </c>
+      <c r="X301" s="3" t="s">
+        <v>1863</v>
+      </c>
+      <c r="Y301" s="3" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="302" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A302" s="3">
+        <v>301</v>
+      </c>
+      <c r="B302" s="3" t="s">
+        <v>1762</v>
+      </c>
+      <c r="C302" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D302" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="E302" s="3" t="s">
+        <v>1763</v>
+      </c>
+      <c r="F302" s="3" t="s">
+        <v>1864</v>
+      </c>
+      <c r="G302" s="3" t="s">
+        <v>1865</v>
+      </c>
+      <c r="H302" s="3" t="s">
+        <v>1866</v>
+      </c>
+      <c r="K302" s="10" t="s">
+        <v>1867</v>
+      </c>
+      <c r="L302" s="3">
+        <v>52.171813999999998</v>
+      </c>
+      <c r="M302" s="3">
+        <v>11.641794000000001</v>
+      </c>
+      <c r="N302" s="3">
+        <v>2007</v>
+      </c>
+      <c r="O302" s="3">
+        <v>2</v>
+      </c>
+      <c r="P302" s="3">
+        <v>18</v>
+      </c>
+      <c r="Q302" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="V302" s="3">
+        <v>1</v>
+      </c>
+      <c r="W302" s="3" t="s">
+        <v>1868</v>
+      </c>
+      <c r="X302" s="3" t="s">
+        <v>1869</v>
+      </c>
+      <c r="Y302" s="3" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="303" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A303" s="3">
+        <v>302</v>
+      </c>
+      <c r="B303" s="3" t="s">
+        <v>1870</v>
+      </c>
+      <c r="C303" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D303" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="E303" s="3" t="s">
+        <v>1763</v>
+      </c>
+      <c r="F303" s="3" t="s">
+        <v>1830</v>
+      </c>
+      <c r="G303" s="3" t="s">
+        <v>1871</v>
+      </c>
+      <c r="H303" s="3" t="s">
+        <v>1872</v>
+      </c>
+      <c r="I303" s="3" t="s">
+        <v>1873</v>
+      </c>
+      <c r="K303" s="10" t="s">
+        <v>1874</v>
+      </c>
+      <c r="L303" s="3">
+        <v>50.883319099999987</v>
+      </c>
+      <c r="M303" s="3">
+        <v>11.61813150165227</v>
+      </c>
+      <c r="N303" s="3">
+        <v>2007</v>
+      </c>
+      <c r="O303" s="3">
+        <v>2</v>
+      </c>
+      <c r="P303" s="3">
+        <v>18</v>
+      </c>
+      <c r="Q303" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="V303" s="3">
+        <v>1</v>
+      </c>
+      <c r="W303" s="3" t="s">
+        <v>1875</v>
+      </c>
+      <c r="X303" s="3" t="s">
+        <v>1876</v>
+      </c>
+      <c r="Y303" s="3" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="304" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A304" s="3">
+        <v>303</v>
+      </c>
+      <c r="B304" s="3" t="s">
+        <v>1877</v>
+      </c>
+      <c r="C304" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D304" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="E304" s="3" t="s">
+        <v>1763</v>
+      </c>
+      <c r="F304" s="3" t="s">
+        <v>1764</v>
+      </c>
+      <c r="G304" s="3" t="s">
+        <v>1765</v>
+      </c>
+      <c r="H304" s="3" t="s">
+        <v>1766</v>
+      </c>
+      <c r="I304" s="3" t="s">
+        <v>1767</v>
+      </c>
+      <c r="J304" s="3" t="s">
+        <v>1774</v>
+      </c>
+      <c r="K304" s="10" t="s">
+        <v>1768</v>
+      </c>
+      <c r="L304" s="3">
+        <v>52.442846994321499</v>
+      </c>
+      <c r="M304" s="3">
+        <v>13.588744934591899</v>
+      </c>
+      <c r="N304" s="3">
+        <v>1977</v>
+      </c>
+      <c r="Q304" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="U304" s="3" t="s">
+        <v>1878</v>
+      </c>
+      <c r="V304" s="3">
+        <v>1</v>
+      </c>
+      <c r="W304" s="3" t="s">
+        <v>1879</v>
+      </c>
+      <c r="X304" s="3" t="s">
+        <v>1880</v>
+      </c>
+      <c r="Y304" s="3" t="s">
+        <v>1881</v>
+      </c>
+    </row>
+    <row r="305" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A305" s="3">
+        <v>304</v>
+      </c>
+      <c r="B305" s="3" t="s">
+        <v>1882</v>
+      </c>
+      <c r="C305" s="3" t="s">
+        <v>801</v>
+      </c>
+      <c r="D305" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="E305" s="3" t="s">
+        <v>1763</v>
+      </c>
+      <c r="F305" s="3" t="s">
+        <v>1764</v>
+      </c>
+      <c r="G305" s="3" t="s">
+        <v>1765</v>
+      </c>
+      <c r="H305" s="3" t="s">
+        <v>1766</v>
+      </c>
+      <c r="K305" s="10" t="s">
+        <v>1768</v>
+      </c>
+      <c r="L305" s="3">
+        <v>52.439979999999998</v>
+      </c>
+      <c r="M305" s="3">
+        <v>13.60249</v>
+      </c>
+      <c r="N305" s="3">
+        <v>1973</v>
+      </c>
+      <c r="Q305" s="3" t="s">
+        <v>685</v>
+      </c>
+      <c r="V305" s="3">
+        <v>1</v>
+      </c>
+      <c r="W305" s="3" t="s">
+        <v>1883</v>
+      </c>
+      <c r="Y305" s="3" t="s">
+        <v>1778</v>
+      </c>
+    </row>
+    <row r="306" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A306" s="3">
+        <v>305</v>
+      </c>
+      <c r="B306" s="3" t="s">
+        <v>1884</v>
+      </c>
+      <c r="C306" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D306" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="E306" s="3" t="s">
+        <v>1763</v>
+      </c>
+      <c r="F306" s="3" t="s">
+        <v>1885</v>
+      </c>
+      <c r="G306" s="3" t="s">
+        <v>1886</v>
+      </c>
+      <c r="H306" s="3" t="s">
+        <v>1887</v>
+      </c>
+      <c r="I306" s="3" t="s">
+        <v>1888</v>
+      </c>
+      <c r="J306" s="3" t="s">
+        <v>1889</v>
+      </c>
+      <c r="K306" s="10" t="s">
+        <v>1890</v>
+      </c>
+      <c r="L306" s="3">
+        <v>51.6574521</v>
+      </c>
+      <c r="M306" s="3">
+        <v>7.2415566</v>
+      </c>
+      <c r="N306" s="3">
+        <v>2009</v>
+      </c>
+      <c r="O306" s="3">
+        <v>7</v>
+      </c>
+      <c r="P306" s="3">
+        <v>27</v>
+      </c>
+      <c r="Q306" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="V306" s="3">
+        <v>1</v>
+      </c>
+      <c r="W306" s="3" t="s">
+        <v>1891</v>
+      </c>
+      <c r="Y306" s="3" t="s">
+        <v>1892</v>
+      </c>
+    </row>
+    <row r="307" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A307" s="3">
+        <v>306</v>
+      </c>
+      <c r="B307" s="3" t="s">
+        <v>1893</v>
+      </c>
+      <c r="C307" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D307" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="E307" s="3" t="s">
+        <v>1763</v>
+      </c>
+      <c r="F307" s="3" t="s">
+        <v>1841</v>
+      </c>
+      <c r="G307" s="3" t="s">
+        <v>1894</v>
+      </c>
+      <c r="H307" s="3" t="s">
+        <v>1895</v>
+      </c>
+      <c r="I307" s="3" t="s">
+        <v>1896</v>
+      </c>
+      <c r="K307" s="10">
+        <v>16831</v>
+      </c>
+      <c r="L307" s="3">
+        <v>53.101875735417302</v>
+      </c>
+      <c r="M307" s="3">
+        <v>12.901845780002001</v>
+      </c>
+      <c r="N307" s="3">
+        <v>2009</v>
+      </c>
+      <c r="O307" s="3">
+        <v>6</v>
+      </c>
+      <c r="P307" s="3">
+        <v>16</v>
+      </c>
+      <c r="Q307" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="V307" s="3">
+        <v>1</v>
+      </c>
+      <c r="X307" s="3" t="s">
+        <v>1897</v>
+      </c>
+      <c r="Y307" s="3" t="s">
+        <v>1898</v>
+      </c>
+    </row>
+    <row r="308" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A308" s="3">
+        <v>307</v>
+      </c>
+      <c r="B308" s="3" t="s">
+        <v>1899</v>
+      </c>
+      <c r="C308" s="3" t="s">
+        <v>1900</v>
+      </c>
+      <c r="D308" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="E308" s="3" t="s">
+        <v>1763</v>
+      </c>
+      <c r="F308" s="3" t="s">
+        <v>1841</v>
+      </c>
+      <c r="G308" s="3" t="s">
+        <v>1901</v>
+      </c>
+      <c r="H308" s="3" t="s">
+        <v>1902</v>
+      </c>
+      <c r="N308" s="3">
+        <v>1979</v>
+      </c>
+      <c r="Q308" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="U308" s="3" t="s">
+        <v>1903</v>
+      </c>
+      <c r="V308" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y308" s="3" t="s">
+        <v>1904</v>
+      </c>
+    </row>
+    <row r="309" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A309" s="3">
+        <v>308</v>
+      </c>
+      <c r="B309" s="3" t="s">
+        <v>1905</v>
+      </c>
+      <c r="C309" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D309" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="E309" s="3" t="s">
+        <v>1763</v>
+      </c>
+      <c r="F309" s="3" t="s">
+        <v>1864</v>
+      </c>
+      <c r="G309" s="3" t="s">
+        <v>1906</v>
+      </c>
+      <c r="H309" s="3" t="s">
+        <v>1907</v>
+      </c>
+      <c r="I309" s="3" t="s">
+        <v>1908</v>
+      </c>
+      <c r="K309" s="10" t="s">
+        <v>1909</v>
+      </c>
+      <c r="L309" s="3">
+        <v>52.626890600000003</v>
+      </c>
+      <c r="M309" s="3">
+        <v>11.175854838090229</v>
+      </c>
+      <c r="N309" s="3">
+        <v>1974</v>
+      </c>
+      <c r="Q309" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="V309" s="3">
+        <v>1</v>
+      </c>
+      <c r="W309" s="3" t="s">
+        <v>1910</v>
+      </c>
+      <c r="X309" s="3" t="s">
+        <v>1911</v>
+      </c>
+      <c r="Y309" s="3" t="s">
+        <v>1912</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="B1:AO286" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="B1:AO309" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="A1">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>

</xml_diff>

<commit_message>
More FR data, work on allende_scraper_france_paris
</commit_message>
<xml_diff>
--- a/a-place-for-salvador-allende/a_place_for_salvador_allende.xlsx
+++ b/a-place-for-salvador-allende/a_place_for_salvador_allende.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GoGro\Desktop\Repos\datasets-of-interest\a-place-for-salvador-allende\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD035165-264E-45F4-90FA-6450E7475D57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E280CD7-5E61-4134-A3A3-470D1E525059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33480" yWindow="2925" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="allende" sheetId="1" r:id="rId1"/>
@@ -7510,7 +7510,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B57" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J91" sqref="J91"/>
+      <selection pane="bottomRight" activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>